<commit_message>
Fixed small data bug and pushed new example and AWS baseline that seems to break this push of the parser.
Signed-off-by: Aaron Lippold <lippold@gmail.com>
</commit_message>
<xml_diff>
--- a/data/NIST_Map_09212017B_CSC-CIS_Critical_Security_Controls_VER_6.1_Excel_9.1.2016.xlsx
+++ b/data/NIST_Map_09212017B_CSC-CIS_Critical_Security_Controls_VER_6.1_Excel_9.1.2016.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\earonne\Desktop\CIS_mapping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaronl/Desktop/hardening/aaronlippold/pdf2inspec/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20160" windowHeight="9312" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20160" windowHeight="9320" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="INTRODUCTION" sheetId="1" r:id="rId1"/>
@@ -23,24 +23,30 @@
     <definedName name="Z_784EFDF6_DF57_4744_A1FE_569B86C0D3A6_.wvu.PrintArea" localSheetId="1" hidden="1">'VER 6.1 Controls'!$C$3:$E$172</definedName>
     <definedName name="Z_9FD8CC1C_6420_44A1_A370_C19CD963FBCC_.wvu.FilterData" localSheetId="1" hidden="1">'VER 6.1 Controls'!$A$3:$H$172</definedName>
     <definedName name="Z_9FD8CC1C_6420_44A1_A370_C19CD963FBCC_.wvu.PrintArea" localSheetId="1" hidden="1">'VER 6.1 Controls'!$C$3:$E$172</definedName>
+    <definedName name="Z_D2DB1628_96BC_634F_B558_28007DD1D3D1_.wvu.FilterData" localSheetId="1" hidden="1">'VER 6.1 Controls'!$A$3:$H$172</definedName>
+    <definedName name="Z_D2DB1628_96BC_634F_B558_28007DD1D3D1_.wvu.PrintArea" localSheetId="1" hidden="1">'VER 6.1 Controls'!$C$3:$E$172</definedName>
     <definedName name="Z_FAFBD161_BACA_2748_AF1F_CDB375FB6AE3_.wvu.PrintArea" localSheetId="1" hidden="1">'VER 6.1 Controls'!$C$3:$E$172</definedName>
     <definedName name="Z_FB597F9D_3EB9_9C48_BC71_4C09FB1B9DF4_.wvu.PrintArea" localSheetId="1" hidden="1">'VER 6.1 Controls'!$C$3:$E$172</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{D2DB1628-96BC-634F-B558-28007DD1D3D1}" mergeInterval="0" personalView="1" windowWidth="1008" windowHeight="293" activeSheetId="2"/>
+    <customWorkbookView name="Robin Regnier - Personal View" guid="{156F6E94-B77C-4218-9566-01A2D0E67E8E}" mergeInterval="0" personalView="1" maximized="1" xWindow="1916" yWindow="-4" windowWidth="1928" windowHeight="1088" activeSheetId="2"/>
+    <customWorkbookView name="Kathryn Burns - Personal View" guid="{FB597F9D-3EB9-9C48-BC71-4C09FB1B9DF4}" mergeInterval="0" personalView="1" xWindow="193" yWindow="54" windowWidth="1280" windowHeight="644" activeSheetId="2"/>
+    <customWorkbookView name="James Tarala - Personal View" guid="{784EFDF6-DF57-4744-A1FE-569B86C0D3A6}" mergeInterval="0" personalView="1" maximized="1" xWindow="-4" yWindow="-4" windowWidth="2168" windowHeight="1404" activeSheetId="2" showComments="commIndAndComment"/>
+    <customWorkbookView name="Tony Sager - Personal View" guid="{FAFBD161-BACA-2748-AF1F-CDB375FB6AE3}" mergeInterval="0" personalView="1" yWindow="54" windowWidth="2560" windowHeight="1295" activeSheetId="2"/>
+    <customWorkbookView name="Haynes, Dan - Personal View" guid="{166C989B-D112-4FBE-9337-483856443AEC}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1918" windowHeight="1030" activeSheetId="2"/>
     <customWorkbookView name="Aronne, Eugene J. - Personal View" guid="{9FD8CC1C-6420-44A1-A370-C19CD963FBCC}" mergeInterval="0" personalView="1" maximized="1" xWindow="-9" yWindow="-9" windowWidth="1938" windowHeight="1064" activeSheetId="2"/>
-    <customWorkbookView name="Haynes, Dan - Personal View" guid="{166C989B-D112-4FBE-9337-483856443AEC}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1918" windowHeight="1030" activeSheetId="2"/>
-    <customWorkbookView name="Tony Sager - Personal View" guid="{FAFBD161-BACA-2748-AF1F-CDB375FB6AE3}" mergeInterval="0" personalView="1" yWindow="54" windowWidth="2560" windowHeight="1295" activeSheetId="2"/>
-    <customWorkbookView name="James Tarala - Personal View" guid="{784EFDF6-DF57-4744-A1FE-569B86C0D3A6}" mergeInterval="0" personalView="1" maximized="1" xWindow="-4" yWindow="-4" windowWidth="2168" windowHeight="1404" activeSheetId="2" showComments="commIndAndComment"/>
-    <customWorkbookView name="Kathryn Burns - Personal View" guid="{FB597F9D-3EB9-9C48-BC71-4C09FB1B9DF4}" mergeInterval="0" personalView="1" xWindow="193" yWindow="54" windowWidth="1280" windowHeight="644" activeSheetId="2"/>
-    <customWorkbookView name="Robin Regnier - Personal View" guid="{156F6E94-B77C-4218-9566-01A2D0E67E8E}" mergeInterval="0" personalView="1" maximized="1" xWindow="1916" yWindow="-4" windowWidth="1928" windowHeight="1088" activeSheetId="2"/>
   </customWorkbookViews>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -1137,9 +1143,6 @@
     <t>IA-3</t>
   </si>
   <si>
-    <t>IA-3(3)</t>
-  </si>
-  <si>
     <t>DEVICE IDENTIFICATION AND AUTHENTICATION | DYNAMIC ADDRESS ALLOCATION</t>
   </si>
   <si>
@@ -1251,69 +1254,21 @@
     <t>LEAST PRIVILEGE</t>
   </si>
   <si>
-    <t>AC-6(9)</t>
-  </si>
-  <si>
     <t>LEAST PRIVILEGE | AUDITING USE OF PRIVILEGED FUNCTIONS</t>
   </si>
   <si>
-    <t>CM-8(3)</t>
-  </si>
-  <si>
-    <t>CM-8(2)</t>
-  </si>
-  <si>
-    <t>IA-3(1)</t>
-  </si>
-  <si>
-    <t>CM-7(5)</t>
-  </si>
-  <si>
-    <t>CM-7(2)</t>
-  </si>
-  <si>
-    <t>CM-2(2)</t>
-  </si>
-  <si>
-    <t>CM-6(1)</t>
-  </si>
-  <si>
-    <t>CM-6(2)</t>
-  </si>
-  <si>
-    <t>SI-4(16)</t>
-  </si>
-  <si>
-    <t>RA-5(5)</t>
-  </si>
-  <si>
-    <t>RA-5(1)</t>
-  </si>
-  <si>
-    <t>RA-5(6)</t>
-  </si>
-  <si>
-    <t>AC-6(7)</t>
-  </si>
-  <si>
     <t>LEAST PRIVILEGE | REVIEW OF USER PRIVILEGES</t>
   </si>
   <si>
     <t>AUTHENTICATOR MANAGEMENT | CHANGE AUTHENTICATORS PRIOR TO DELIVERY</t>
   </si>
   <si>
-    <t>IA-5(5)</t>
-  </si>
-  <si>
     <t>AC-2(12)</t>
   </si>
   <si>
     <t>ACCOUNT MANAGEMENT | ACCOUNT MONITORING / ATYPICAL USAGE</t>
   </si>
   <si>
-    <t>AC-2(4)</t>
-  </si>
-  <si>
     <t>ACCOUNT MANAGEMENT | AUTOMATED AUDIT ACTIONS</t>
   </si>
   <si>
@@ -1326,18 +1281,9 @@
     <t>IDENTIFICATION AND AUTHENTICATION | NETWORK ACCESS TO PRIVILEGED ACCOUNTS</t>
   </si>
   <si>
-    <t>IA-2(1)</t>
-  </si>
-  <si>
-    <t>IA-5(1)</t>
-  </si>
-  <si>
     <t>AUTHENTICATOR MANAGEMENT | PASSWORD-BASED AUTHENTICATION</t>
   </si>
   <si>
-    <t>IA-5(8)</t>
-  </si>
-  <si>
     <t>AUTHENTICATOR MANAGEMENT | MULTIPLE INFORMATION SYSTEM ACCOUNTS</t>
   </si>
   <si>
@@ -1350,9 +1296,6 @@
     <t>AU-6</t>
   </si>
   <si>
-    <t>AU-8(2)</t>
-  </si>
-  <si>
     <t>TIME STAMPS | SECONDARY AUTHORITATIVE TIME SOURCE</t>
   </si>
   <si>
@@ -1377,13 +1320,7 @@
     <t>INFORMATION SYSTEM MONITORING | INBOUND AND OUTBOUND COMMUNICATIONS TRAFFIC</t>
   </si>
   <si>
-    <t>SI-4(4)</t>
-  </si>
-  <si>
     <t>INFORMATION SYSTEM MONITORING | AUTOMATED TOOLS FOR REAL-TIME ANALYSIS</t>
-  </si>
-  <si>
-    <t>SI-4(2)</t>
   </si>
   <si>
     <t>SC-7</t>
@@ -1525,9 +1462,6 @@
     <t>SC-7(5)</t>
   </si>
   <si>
-    <t>CM-7(1)</t>
-  </si>
-  <si>
     <t>SI-10</t>
   </si>
   <si>
@@ -1537,9 +1471,6 @@
     <t>INFORMATION SYSTEM BACKUP | TESTING FOR RELIABILITY / INTEGRITY</t>
   </si>
   <si>
-    <t>CP-9(1)</t>
-  </si>
-  <si>
     <t>INFORMATION SYSTEM BACKUP | SEPARATE STORAGE FOR CRITICAL INFORMATION</t>
   </si>
   <si>
@@ -1555,15 +1486,9 @@
     <t>INFORMATION SYSTEM COMPONENT INVENTORY | ASSESSED CONFIGURATIONS / APPROVED DEVIATIONS</t>
   </si>
   <si>
-    <t>CM-8(6)</t>
-  </si>
-  <si>
     <t>PENETRATION TESTING | RED TEAM EXERCISES</t>
   </si>
   <si>
-    <t>CA-8(2)</t>
-  </si>
-  <si>
     <t>INCIDENT RESPONSE TRAINING</t>
   </si>
   <si>
@@ -1585,9 +1510,6 @@
     <t>INFORMATION SYSTEM MONITORING | WIRELESS INTRUSION DETECTION</t>
   </si>
   <si>
-    <t>SI-4(14)</t>
-  </si>
-  <si>
     <t>PERSONNEL TERMINATION</t>
   </si>
   <si>
@@ -1618,15 +1540,9 @@
     <t>WIRELESS ACCESS | AUTHENTICATION AND ENCRYPTION</t>
   </si>
   <si>
-    <t>AC-18(1)</t>
-  </si>
-  <si>
     <t>AUDIT REVIEW, ANALYSIS, AND REPORTING | INTEGRATION / SCANNING AND MONITORING CAPABILITIES</t>
   </si>
   <si>
-    <t>AU-6(5)</t>
-  </si>
-  <si>
     <t>IA-2</t>
   </si>
   <si>
@@ -1648,39 +1564,21 @@
     <t>SYSTEM INTERCONNECTIONS | RESTRICTIONS ON EXTERNAL SYSTEM CONNECTIONS</t>
   </si>
   <si>
-    <t>CA-3(5)</t>
-  </si>
-  <si>
     <t>INFORMATION SYSTEM MONITORING | SYSTEM-WIDE INTRUSION DETECTION SYSTEM</t>
   </si>
   <si>
-    <t>SI-4(1)</t>
-  </si>
-  <si>
     <t>BOUNDARY PROTECTION | ROUTE TRAFFIC TO AUTHENTICATED PROXY SERVERS</t>
   </si>
   <si>
-    <t>SC-7(8)</t>
-  </si>
-  <si>
     <t>DEVICE IDENTIFICATION AND AUTHENTICATION | DEVICE ATTESTATION</t>
   </si>
   <si>
-    <t>IA-3(4)</t>
-  </si>
-  <si>
     <t>INFORMATION SYSTEM MONITORING | ANALYZE COMMUNICATIONS TRAFFIC ANOMALIES</t>
   </si>
   <si>
-    <t>SI-4(11)</t>
-  </si>
-  <si>
     <t>INFORMATION SYSTEM MONITORING | ANALYZE TRAFFIC / COVERT EXFILTRATION</t>
   </si>
   <si>
-    <t>SI-4(18)</t>
-  </si>
-  <si>
     <t>PRIVACY IMPACT AND RISK ASSESSMENT</t>
   </si>
   <si>
@@ -1690,21 +1588,12 @@
     <t>PROTECTION OF INFORMATION AT REST | CRYPTOGRAPHIC PROTECTION</t>
   </si>
   <si>
-    <t>SC-28(1)</t>
-  </si>
-  <si>
     <t>BOUNDARY PROTECTION | PREVENT UNAUTHORIZED EXFILTRATION</t>
   </si>
   <si>
-    <t>SC-7(10)</t>
-  </si>
-  <si>
     <t>MINIMIZATION OF PERSONALLY IDENTIFIABLE INFORMATION | LOCATE / REMOVE / REDACT / ANONYMIZE PII</t>
   </si>
   <si>
-    <t>DM-1(1)</t>
-  </si>
-  <si>
     <t>MP-4</t>
   </si>
   <si>
@@ -1714,13 +1603,130 @@
     <t>INFORMATION FLOW ENFORCEMENT | CONTENT CHECK ENCRYPTED INFORMATION</t>
   </si>
   <si>
-    <t>AC-4(4)</t>
+    <t>CM-8 (3)</t>
+  </si>
+  <si>
+    <t>IA-3 (3)</t>
+  </si>
+  <si>
+    <t>CM-8 (2)</t>
+  </si>
+  <si>
+    <t>IA-3 (1)</t>
+  </si>
+  <si>
+    <t>CM-7 (5)</t>
+  </si>
+  <si>
+    <t>CM-7 (2)</t>
+  </si>
+  <si>
+    <t>CM-2 (2)</t>
+  </si>
+  <si>
+    <t>CM-6 (1)</t>
+  </si>
+  <si>
+    <t>CM-6 (2)</t>
+  </si>
+  <si>
+    <t>SI-4 (16)</t>
+  </si>
+  <si>
+    <t>RA-5 (5)</t>
+  </si>
+  <si>
+    <t>RA-5 (1)</t>
+  </si>
+  <si>
+    <t>AU-6 (5)</t>
+  </si>
+  <si>
+    <t>RA-5 (6)</t>
+  </si>
+  <si>
+    <t>AC-6 (9)</t>
+  </si>
+  <si>
+    <t>AC-6 (7)</t>
+  </si>
+  <si>
+    <t>IA-5 (5)</t>
+  </si>
+  <si>
+    <t>AC-2 (4)</t>
+  </si>
+  <si>
+    <t>IA-2 (1)</t>
+  </si>
+  <si>
+    <t>IA-5 (1)</t>
+  </si>
+  <si>
+    <t>IA-5 (8)</t>
+  </si>
+  <si>
+    <t>AU-8 (2)</t>
+  </si>
+  <si>
+    <t>SI-4 (4)</t>
+  </si>
+  <si>
+    <t>SI-4 (2)</t>
+  </si>
+  <si>
+    <t>CM-7 (1)</t>
+  </si>
+  <si>
+    <t>CP-9 (1)</t>
+  </si>
+  <si>
+    <t>CM-8 (6)</t>
+  </si>
+  <si>
+    <t>CA-3 (5)</t>
+  </si>
+  <si>
+    <t>SI-4 (1)</t>
+  </si>
+  <si>
+    <t>SC-7 (8)</t>
+  </si>
+  <si>
+    <t>IA-3 (4)</t>
+  </si>
+  <si>
+    <t>SI-4 (11)</t>
+  </si>
+  <si>
+    <t>SI-4 (18)</t>
+  </si>
+  <si>
+    <t>SC-28 (1)</t>
+  </si>
+  <si>
+    <t>SC-7 (10)</t>
+  </si>
+  <si>
+    <t>DM-1 (1)</t>
+  </si>
+  <si>
+    <t>AC-4 (4)</t>
+  </si>
+  <si>
+    <t>SI-4 (14)</t>
+  </si>
+  <si>
+    <t>AC-18 (1)</t>
+  </si>
+  <si>
+    <t>CA-8 (2)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1947,16 +1953,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2177,7 +2183,7 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{6663B3B2-0172-4D31-B8DB-D15A051B9192}" diskRevisions="1" revisionId="810" version="9">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{2F8F7620-4C4F-A040-A1DD-B07BF2744515}" diskRevisions="1" revisionId="863" version="10">
   <header guid="{5EC76917-8FE5-4B58-BD6B-154862C439F5}" dateTime="2017-09-20T09:12:56" maxSheetId="3" userName="Haynes, Dan" r:id="rId33">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -2346,6 +2352,12 @@
       <sheetId val="2"/>
     </sheetIdMap>
   </header>
+  <header guid="{2F8F7620-4C4F-A040-A1DD-B07BF2744515}" dateTime="2017-09-28T11:13:57" maxSheetId="3" userName="Microsoft Office User" r:id="rId61" minRId="811" maxRId="861">
+    <sheetIdMap count="2">
+      <sheetId val="1"/>
+      <sheetId val="2"/>
+    </sheetIdMap>
+  </header>
 </headers>
 </file>
 
@@ -5983,6 +5995,630 @@
     <oldFormula>'VER 6.1 Controls'!$A$3:$H$172</oldFormula>
   </rdn>
   <rcv guid="{9FD8CC1C-6420-44A1-A370-C19CD963FBCC}" action="add"/>
+</revisions>
+</file>
+
+<file path=xl/revisions/revisionLog29.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="811" sId="2">
+    <oc r="A5" t="inlineStr">
+      <is>
+        <t>CM-8(3)</t>
+      </is>
+    </oc>
+    <nc r="A5" t="inlineStr">
+      <is>
+        <t>CM-8 (3)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="812" sId="2">
+    <oc r="A6" t="inlineStr">
+      <is>
+        <t>IA-3(3)</t>
+      </is>
+    </oc>
+    <nc r="A6" t="inlineStr">
+      <is>
+        <t>IA-3 (3)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="813" sId="2">
+    <oc r="A7" t="inlineStr">
+      <is>
+        <t>CM-8(2)</t>
+      </is>
+    </oc>
+    <nc r="A7" t="inlineStr">
+      <is>
+        <t>CM-8 (2)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="814" sId="2">
+    <oc r="A10" t="inlineStr">
+      <is>
+        <t>IA-3(1)</t>
+      </is>
+    </oc>
+    <nc r="A10" t="inlineStr">
+      <is>
+        <t>IA-3 (1)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="815" sId="2">
+    <oc r="A12" t="inlineStr">
+      <is>
+        <t>CM-7(5)</t>
+      </is>
+    </oc>
+    <nc r="A12" t="inlineStr">
+      <is>
+        <t>CM-7 (5)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="816" sId="2">
+    <oc r="A13" t="inlineStr">
+      <is>
+        <t>CM-7(2)</t>
+      </is>
+    </oc>
+    <nc r="A13" t="inlineStr">
+      <is>
+        <t>CM-7 (2)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="817" sId="2">
+    <oc r="A14" t="inlineStr">
+      <is>
+        <t>CM-2(2)</t>
+      </is>
+    </oc>
+    <nc r="A14" t="inlineStr">
+      <is>
+        <t>CM-2 (2)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="818" sId="2">
+    <oc r="A19" t="inlineStr">
+      <is>
+        <t>CM-2(2)</t>
+      </is>
+    </oc>
+    <nc r="A19" t="inlineStr">
+      <is>
+        <t>CM-2 (2)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="819" sId="2">
+    <oc r="A22" t="inlineStr">
+      <is>
+        <t>CM-6(1)</t>
+      </is>
+    </oc>
+    <nc r="A22" t="inlineStr">
+      <is>
+        <t>CM-6 (1)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="820" sId="2">
+    <oc r="A23" t="inlineStr">
+      <is>
+        <t>CM-6(2)</t>
+      </is>
+    </oc>
+    <nc r="A23" t="inlineStr">
+      <is>
+        <t>CM-6 (2)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="821" sId="2">
+    <oc r="A26" t="inlineStr">
+      <is>
+        <t>SI-4(16)</t>
+      </is>
+    </oc>
+    <nc r="A26" t="inlineStr">
+      <is>
+        <t>SI-4 (16)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="822" sId="2">
+    <oc r="A27" t="inlineStr">
+      <is>
+        <t>RA-5(5)</t>
+      </is>
+    </oc>
+    <nc r="A27" t="inlineStr">
+      <is>
+        <t>RA-5 (5)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="823" sId="2">
+    <oc r="A28" t="inlineStr">
+      <is>
+        <t>RA-5(1)</t>
+      </is>
+    </oc>
+    <nc r="A28" t="inlineStr">
+      <is>
+        <t>RA-5 (1)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="824" sId="2">
+    <oc r="A30" t="inlineStr">
+      <is>
+        <t>AU-6(5)</t>
+      </is>
+    </oc>
+    <nc r="A30" t="inlineStr">
+      <is>
+        <t>AU-6 (5)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="825" sId="2">
+    <oc r="A31" t="inlineStr">
+      <is>
+        <t>RA-5(6)</t>
+      </is>
+    </oc>
+    <nc r="A31" t="inlineStr">
+      <is>
+        <t>RA-5 (6)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="826" sId="2">
+    <oc r="A34" t="inlineStr">
+      <is>
+        <t>AC-6(9)</t>
+      </is>
+    </oc>
+    <nc r="A34" t="inlineStr">
+      <is>
+        <t>AC-6 (9)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="827" sId="2">
+    <oc r="A35" t="inlineStr">
+      <is>
+        <t>AC-6(7)</t>
+      </is>
+    </oc>
+    <nc r="A35" t="inlineStr">
+      <is>
+        <t>AC-6 (7)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="828" sId="2">
+    <oc r="A36" t="inlineStr">
+      <is>
+        <t>IA-5(5)</t>
+      </is>
+    </oc>
+    <nc r="A36" t="inlineStr">
+      <is>
+        <t>IA-5 (5)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="829" sId="2">
+    <oc r="A37" t="inlineStr">
+      <is>
+        <t>AC-2(4)</t>
+      </is>
+    </oc>
+    <nc r="A37" t="inlineStr">
+      <is>
+        <t>AC-2 (4)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="830" sId="2">
+    <oc r="A39" t="inlineStr">
+      <is>
+        <t>IA-2(1)</t>
+      </is>
+    </oc>
+    <nc r="A39" t="inlineStr">
+      <is>
+        <t>IA-2 (1)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="831" sId="2">
+    <oc r="A40" t="inlineStr">
+      <is>
+        <t>IA-5(1)</t>
+      </is>
+    </oc>
+    <nc r="A40" t="inlineStr">
+      <is>
+        <t>IA-5 (1)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="832" sId="2">
+    <oc r="A41" t="inlineStr">
+      <is>
+        <t>IA-5(8)</t>
+      </is>
+    </oc>
+    <nc r="A41" t="inlineStr">
+      <is>
+        <t>IA-5 (8)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="833" sId="2">
+    <oc r="A44" t="inlineStr">
+      <is>
+        <t>AU-8(2)</t>
+      </is>
+    </oc>
+    <nc r="A44" t="inlineStr">
+      <is>
+        <t>AU-8 (2)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="834" sId="2">
+    <oc r="A48" t="inlineStr">
+      <is>
+        <t>SI-4(4)</t>
+      </is>
+    </oc>
+    <nc r="A48" t="inlineStr">
+      <is>
+        <t>SI-4 (4)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="835" sId="2">
+    <oc r="A49" t="inlineStr">
+      <is>
+        <t>SI-4(2)</t>
+      </is>
+    </oc>
+    <nc r="A49" t="inlineStr">
+      <is>
+        <t>SI-4 (2)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="836" sId="2">
+    <oc r="A67" t="inlineStr">
+      <is>
+        <t>CM-7(1)</t>
+      </is>
+    </oc>
+    <nc r="A67" t="inlineStr">
+      <is>
+        <t>CM-7 (1)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="837" sId="2">
+    <oc r="A75" t="inlineStr">
+      <is>
+        <t>CP-9(1)</t>
+      </is>
+    </oc>
+    <nc r="A75" t="inlineStr">
+      <is>
+        <t>CP-9 (1)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="838" sId="2">
+    <oc r="A79" t="inlineStr">
+      <is>
+        <t>CM-6(1)</t>
+      </is>
+    </oc>
+    <nc r="A79" t="inlineStr">
+      <is>
+        <t>CM-6 (1)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="839" sId="2">
+    <oc r="A80" t="inlineStr">
+      <is>
+        <t>CM-8(6)</t>
+      </is>
+    </oc>
+    <nc r="A80" t="inlineStr">
+      <is>
+        <t>CM-8 (6)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="840" sId="2">
+    <oc r="A81" t="inlineStr">
+      <is>
+        <t>CM-6(2)</t>
+      </is>
+    </oc>
+    <nc r="A81" t="inlineStr">
+      <is>
+        <t>CM-6 (2)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="841" sId="2">
+    <oc r="A87" t="inlineStr">
+      <is>
+        <t>CA-3(5)</t>
+      </is>
+    </oc>
+    <nc r="A87" t="inlineStr">
+      <is>
+        <t>CA-3 (5)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="842" sId="2">
+    <oc r="A88" t="inlineStr">
+      <is>
+        <t>SI-4(2)</t>
+      </is>
+    </oc>
+    <nc r="A88" t="inlineStr">
+      <is>
+        <t>SI-4 (2)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="843" sId="2">
+    <oc r="A89" t="inlineStr">
+      <is>
+        <t>SI-4(1)</t>
+      </is>
+    </oc>
+    <nc r="A89" t="inlineStr">
+      <is>
+        <t>SI-4 (1)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="844" sId="2">
+    <oc r="A91" t="inlineStr">
+      <is>
+        <t>SC-7(8)</t>
+      </is>
+    </oc>
+    <nc r="A91" t="inlineStr">
+      <is>
+        <t>SC-7 (8)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="845" sId="2">
+    <oc r="A92" t="inlineStr">
+      <is>
+        <t>IA-2(1)</t>
+      </is>
+    </oc>
+    <nc r="A92" t="inlineStr">
+      <is>
+        <t>IA-2 (1)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="846" sId="2">
+    <oc r="A93" t="inlineStr">
+      <is>
+        <t>IA-3(4)</t>
+      </is>
+    </oc>
+    <nc r="A93" t="inlineStr">
+      <is>
+        <t>IA-3 (4)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="847" sId="2">
+    <oc r="A95" t="inlineStr">
+      <is>
+        <t>SI-4(11)</t>
+      </is>
+    </oc>
+    <nc r="A95" t="inlineStr">
+      <is>
+        <t>SI-4 (11)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="848" sId="2">
+    <oc r="A96" t="inlineStr">
+      <is>
+        <t>SI-4(18)</t>
+      </is>
+    </oc>
+    <nc r="A96" t="inlineStr">
+      <is>
+        <t>SI-4 (18)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="849" sId="2">
+    <oc r="A99" t="inlineStr">
+      <is>
+        <t>SC-28(1)</t>
+      </is>
+    </oc>
+    <nc r="A99" t="inlineStr">
+      <is>
+        <t>SC-28 (1)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="850" sId="2">
+    <oc r="A100" t="inlineStr">
+      <is>
+        <t>SC-7(10)</t>
+      </is>
+    </oc>
+    <nc r="A100" t="inlineStr">
+      <is>
+        <t>SC-7 (10)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="851" sId="2">
+    <oc r="A101" t="inlineStr">
+      <is>
+        <t>DM-1(1)</t>
+      </is>
+    </oc>
+    <nc r="A101" t="inlineStr">
+      <is>
+        <t>DM-1 (1)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="852" sId="2">
+    <oc r="A103" t="inlineStr">
+      <is>
+        <t>SI-4(4)</t>
+      </is>
+    </oc>
+    <nc r="A103" t="inlineStr">
+      <is>
+        <t>SI-4 (4)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="853" sId="2">
+    <oc r="A104" t="inlineStr">
+      <is>
+        <t>AC-4(4)</t>
+      </is>
+    </oc>
+    <nc r="A104" t="inlineStr">
+      <is>
+        <t>AC-4 (4)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="854" sId="2">
+    <oc r="A105" t="inlineStr">
+      <is>
+        <t>SC-7(10)</t>
+      </is>
+    </oc>
+    <nc r="A105" t="inlineStr">
+      <is>
+        <t>SC-7 (10)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="855" sId="2">
+    <oc r="A117" t="inlineStr">
+      <is>
+        <t>SI-4(14)</t>
+      </is>
+    </oc>
+    <nc r="A117" t="inlineStr">
+      <is>
+        <t>SI-4 (14)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="856" sId="2">
+    <oc r="A118" t="inlineStr">
+      <is>
+        <t>SI-4(14)</t>
+      </is>
+    </oc>
+    <nc r="A118" t="inlineStr">
+      <is>
+        <t>SI-4 (14)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="857" sId="2">
+    <oc r="A120" t="inlineStr">
+      <is>
+        <t>AC-18(1)</t>
+      </is>
+    </oc>
+    <nc r="A120" t="inlineStr">
+      <is>
+        <t>AC-18 (1)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="858" sId="2">
+    <oc r="A121" t="inlineStr">
+      <is>
+        <t>AC-18(1)</t>
+      </is>
+    </oc>
+    <nc r="A121" t="inlineStr">
+      <is>
+        <t>AC-18 (1)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="859" sId="2">
+    <oc r="A136" t="inlineStr">
+      <is>
+        <t>IA-2(1)</t>
+      </is>
+    </oc>
+    <nc r="A136" t="inlineStr">
+      <is>
+        <t>IA-2 (1)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="860" sId="2">
+    <oc r="A167" t="inlineStr">
+      <is>
+        <t>CA-8(2)</t>
+      </is>
+    </oc>
+    <nc r="A167" t="inlineStr">
+      <is>
+        <t>CA-8 (2)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rcc rId="861" sId="2">
+    <oc r="A171" t="inlineStr">
+      <is>
+        <t>CA-8(2)</t>
+      </is>
+    </oc>
+    <nc r="A171" t="inlineStr">
+      <is>
+        <t>CA-8 (2)</t>
+      </is>
+    </nc>
+  </rcc>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_D2DB1628_96BC_634F_B558_28007DD1D3D1_.wvu.PrintArea" hidden="1" oldHidden="1">
+    <formula>'VER 6.1 Controls'!$C$3:$E$172</formula>
+  </rdn>
+  <rdn rId="0" localSheetId="2" customView="1" name="Z_D2DB1628_96BC_634F_B558_28007DD1D3D1_.wvu.FilterData" hidden="1" oldHidden="1">
+    <formula>'VER 6.1 Controls'!$A$3:$H$172</formula>
+  </rdn>
+  <rcv guid="{D2DB1628-96BC-634F-B558-28007DD1D3D1}" action="add"/>
 </revisions>
 </file>
 
@@ -6383,51 +7019,51 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="101" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:1" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
     </row>
-    <row r="6" spans="1:1" ht="45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>327</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="5"/>
     </row>
-    <row r="8" spans="1:1" ht="135" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" ht="128" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>324</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{9FD8CC1C-6420-44A1-A370-C19CD963FBCC}">
+    <customSheetView guid="{D2DB1628-96BC-634F-B558-28007DD1D3D1}">
       <selection activeCell="A3" sqref="A3"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{166C989B-D112-4FBE-9337-483856443AEC}">
+    <customSheetView guid="{156F6E94-B77C-4218-9566-01A2D0E67E8E}">
       <selection activeCell="A3" sqref="A3"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{FAFBD161-BACA-2748-AF1F-CDB375FB6AE3}">
-      <selection activeCell="A4" sqref="A4"/>
+    <customSheetView guid="{FB597F9D-3EB9-9C48-BC71-4C09FB1B9DF4}">
+      <selection activeCell="A3" sqref="A3"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
@@ -6436,12 +7072,17 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{FB597F9D-3EB9-9C48-BC71-4C09FB1B9DF4}">
-      <selection activeCell="A3" sqref="A3"/>
+    <customSheetView guid="{FAFBD161-BACA-2748-AF1F-CDB375FB6AE3}">
+      <selection activeCell="A4" sqref="A4"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{156F6E94-B77C-4218-9566-01A2D0E67E8E}">
+    <customSheetView guid="{166C989B-D112-4FBE-9337-483856443AEC}">
+      <selection activeCell="A3" sqref="A3"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{9FD8CC1C-6420-44A1-A370-C19CD963FBCC}">
       <selection activeCell="A3" sqref="A3"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -6449,39 +7090,34 @@
   </customSheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H172"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="A172" sqref="A172"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" customWidth="1"/>
-    <col min="2" max="2" width="41.5546875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5" customWidth="1"/>
+    <col min="2" max="2" width="41.5" style="6" customWidth="1"/>
+    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" customWidth="1"/>
-    <col min="5" max="5" width="68.109375" style="7" customWidth="1"/>
-    <col min="6" max="6" width="15.77734375" customWidth="1"/>
-    <col min="7" max="7" width="17.77734375" customWidth="1"/>
-    <col min="8" max="8" width="30.5546875" style="9" customWidth="1"/>
+    <col min="5" max="5" width="68.1640625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" customWidth="1"/>
+    <col min="7" max="7" width="17.83203125" customWidth="1"/>
+    <col min="8" max="8" width="30.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A1" s="11"/>
       <c r="B1" s="12"/>
       <c r="C1" s="11"/>
@@ -6492,7 +7128,7 @@
       <c r="F1" s="11"/>
       <c r="G1" s="11"/>
     </row>
-    <row r="2" spans="1:7" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="24" x14ac:dyDescent="0.2">
       <c r="A2" s="11"/>
       <c r="B2" s="12"/>
       <c r="C2" s="11"/>
@@ -6503,12 +7139,12 @@
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
     </row>
-    <row r="3" spans="1:7" ht="36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="38" x14ac:dyDescent="0.2">
       <c r="A3" s="14" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>117</v>
@@ -6526,12 +7162,12 @@
         <v>330</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>344</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C4" s="49" t="s">
         <v>0</v>
@@ -6541,12 +7177,12 @@
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
     </row>
-    <row r="5" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
-        <v>386</v>
+        <v>495</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C5" s="17" t="s">
         <v>118</v>
@@ -6564,12 +7200,12 @@
         <v>332</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
+        <v>496</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>346</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>347</v>
       </c>
       <c r="C6" s="17" t="s">
         <v>118</v>
@@ -6585,12 +7221,12 @@
       </c>
       <c r="G6" s="23"/>
     </row>
-    <row r="7" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>387</v>
+        <v>497</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C7" s="17" t="s">
         <v>118</v>
@@ -6606,12 +7242,12 @@
       </c>
       <c r="G7" s="23"/>
     </row>
-    <row r="8" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="165" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>344</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C8" s="17" t="s">
         <v>118</v>
@@ -6627,12 +7263,12 @@
       </c>
       <c r="G8" s="23"/>
     </row>
-    <row r="9" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="75" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>345</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>118</v>
@@ -6650,12 +7286,12 @@
         <v>333</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
-        <v>388</v>
+        <v>498</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C10" s="17" t="s">
         <v>118</v>
@@ -6671,12 +7307,12 @@
         <v>331</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
+        <v>361</v>
+      </c>
+      <c r="B11" s="18" t="s">
         <v>362</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>363</v>
       </c>
       <c r="C11" s="49" t="s">
         <v>4</v>
@@ -6686,12 +7322,12 @@
       <c r="F11" s="11"/>
       <c r="G11" s="11"/>
     </row>
-    <row r="12" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
-        <v>389</v>
+        <v>499</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C12" s="17" t="s">
         <v>118</v>
@@ -6709,12 +7345,12 @@
         <v>334</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="90" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
-        <v>390</v>
+        <v>500</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>118</v>
@@ -6732,12 +7368,12 @@
         <v>335</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="90" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
-        <v>391</v>
+        <v>501</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>118</v>
@@ -6755,12 +7391,12 @@
         <v>336</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>118</v>
@@ -6776,12 +7412,12 @@
         <v>331</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B16" s="18" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C16" s="49" t="s">
         <v>7</v>
@@ -6791,12 +7427,12 @@
       <c r="F16" s="11"/>
       <c r="G16" s="11"/>
     </row>
-    <row r="17" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="75" x14ac:dyDescent="0.2">
       <c r="A17" s="17" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B17" s="18" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C17" s="17" t="s">
         <v>118</v>
@@ -6812,12 +7448,12 @@
       </c>
       <c r="G17" s="28"/>
     </row>
-    <row r="18" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="90" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C18" s="17" t="s">
         <v>118</v>
@@ -6833,12 +7469,12 @@
       </c>
       <c r="G18" s="28"/>
     </row>
-    <row r="19" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="90" x14ac:dyDescent="0.2">
       <c r="A19" s="17" t="s">
-        <v>391</v>
+        <v>501</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C19" s="17" t="s">
         <v>118</v>
@@ -6856,12 +7492,12 @@
         <v>337</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="60" x14ac:dyDescent="0.2">
       <c r="A20" s="17" t="s">
+        <v>365</v>
+      </c>
+      <c r="B20" s="18" t="s">
         <v>366</v>
-      </c>
-      <c r="B20" s="18" t="s">
-        <v>367</v>
       </c>
       <c r="C20" s="17" t="s">
         <v>118</v>
@@ -6877,12 +7513,12 @@
       </c>
       <c r="G20" s="28"/>
     </row>
-    <row r="21" spans="1:7" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="165" x14ac:dyDescent="0.2">
       <c r="A21" s="17" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="C21" s="17" t="s">
         <v>118</v>
@@ -6900,12 +7536,12 @@
         <v>338</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="90" x14ac:dyDescent="0.2">
       <c r="A22" s="17" t="s">
-        <v>392</v>
+        <v>502</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C22" s="17" t="s">
         <v>118</v>
@@ -6921,12 +7557,12 @@
       </c>
       <c r="G22" s="28"/>
     </row>
-    <row r="23" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="75" x14ac:dyDescent="0.2">
       <c r="A23" s="17" t="s">
-        <v>393</v>
+        <v>503</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C23" s="17" t="s">
         <v>118</v>
@@ -6942,12 +7578,12 @@
       </c>
       <c r="G23" s="26"/>
     </row>
-    <row r="24" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
+        <v>371</v>
+      </c>
+      <c r="B24" s="18" t="s">
         <v>372</v>
-      </c>
-      <c r="B24" s="18" t="s">
-        <v>373</v>
       </c>
       <c r="C24" s="49" t="s">
         <v>11</v>
@@ -6957,12 +7593,12 @@
       <c r="F24" s="11"/>
       <c r="G24" s="11"/>
     </row>
-    <row r="25" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="120" x14ac:dyDescent="0.2">
       <c r="A25" s="17" t="s">
+        <v>371</v>
+      </c>
+      <c r="B25" s="18" t="s">
         <v>372</v>
-      </c>
-      <c r="B25" s="18" t="s">
-        <v>373</v>
       </c>
       <c r="C25" s="17" t="s">
         <v>118</v>
@@ -6980,12 +7616,12 @@
         <v>339</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="75" x14ac:dyDescent="0.2">
       <c r="A26" s="17" t="s">
-        <v>394</v>
+        <v>504</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C26" s="17" t="s">
         <v>118</v>
@@ -7001,12 +7637,12 @@
       </c>
       <c r="G26" s="30"/>
     </row>
-    <row r="27" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="105" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
-        <v>395</v>
+        <v>505</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C27" s="17" t="s">
         <v>118</v>
@@ -7022,12 +7658,12 @@
       </c>
       <c r="G27" s="30"/>
     </row>
-    <row r="28" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="75" x14ac:dyDescent="0.2">
       <c r="A28" s="17" t="s">
-        <v>396</v>
+        <v>506</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="C28" s="17" t="s">
         <v>118</v>
@@ -7043,12 +7679,12 @@
       </c>
       <c r="G28" s="30"/>
     </row>
-    <row r="29" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A29" s="17" t="s">
+        <v>377</v>
+      </c>
+      <c r="B29" s="18" t="s">
         <v>378</v>
-      </c>
-      <c r="B29" s="18" t="s">
-        <v>379</v>
       </c>
       <c r="C29" s="17" t="s">
         <v>118</v>
@@ -7064,12 +7700,12 @@
       </c>
       <c r="G29" s="30"/>
     </row>
-    <row r="30" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A30" s="31" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
       <c r="B30" s="32" t="s">
-        <v>503</v>
+        <v>474</v>
       </c>
       <c r="C30" s="17" t="s">
         <v>118</v>
@@ -7085,12 +7721,12 @@
       </c>
       <c r="G30" s="30"/>
     </row>
-    <row r="31" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="90" x14ac:dyDescent="0.2">
       <c r="A31" s="17" t="s">
-        <v>397</v>
+        <v>508</v>
       </c>
       <c r="B31" s="18" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C31" s="17" t="s">
         <v>118</v>
@@ -7106,12 +7742,12 @@
       </c>
       <c r="G31" s="30"/>
     </row>
-    <row r="32" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="75" x14ac:dyDescent="0.2">
       <c r="A32" s="17" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C32" s="17" t="s">
         <v>118</v>
@@ -7127,12 +7763,12 @@
       </c>
       <c r="G32" s="30"/>
     </row>
-    <row r="33" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A33" s="17" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B33" s="18" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C33" s="49" t="s">
         <v>121</v>
@@ -7142,12 +7778,12 @@
       <c r="F33" s="11"/>
       <c r="G33" s="11"/>
     </row>
-    <row r="34" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A34" s="17" t="s">
-        <v>384</v>
+        <v>509</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C34" s="17" t="s">
         <v>118</v>
@@ -7163,12 +7799,12 @@
       </c>
       <c r="G34" s="30"/>
     </row>
-    <row r="35" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
-        <v>398</v>
+        <v>510</v>
       </c>
       <c r="B35" s="18" t="s">
-        <v>399</v>
+        <v>384</v>
       </c>
       <c r="C35" s="17" t="s">
         <v>118</v>
@@ -7184,12 +7820,12 @@
       </c>
       <c r="G35" s="30"/>
     </row>
-    <row r="36" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A36" s="17" t="s">
-        <v>401</v>
+        <v>511</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>400</v>
+        <v>385</v>
       </c>
       <c r="C36" s="17" t="s">
         <v>118</v>
@@ -7205,12 +7841,12 @@
       </c>
       <c r="G36" s="30"/>
     </row>
-    <row r="37" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
-        <v>404</v>
+        <v>512</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>405</v>
+        <v>388</v>
       </c>
       <c r="C37" s="17" t="s">
         <v>118</v>
@@ -7226,12 +7862,12 @@
       </c>
       <c r="G37" s="30"/>
     </row>
-    <row r="38" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
-        <v>406</v>
+        <v>389</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>407</v>
+        <v>390</v>
       </c>
       <c r="C38" s="17" t="s">
         <v>118</v>
@@ -7247,12 +7883,12 @@
       </c>
       <c r="G38" s="30"/>
     </row>
-    <row r="39" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" ht="60" x14ac:dyDescent="0.2">
       <c r="A39" s="17" t="s">
-        <v>409</v>
+        <v>513</v>
       </c>
       <c r="B39" s="18" t="s">
-        <v>408</v>
+        <v>391</v>
       </c>
       <c r="C39" s="17" t="s">
         <v>118</v>
@@ -7268,12 +7904,12 @@
       </c>
       <c r="G39" s="30"/>
     </row>
-    <row r="40" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" s="17" t="s">
-        <v>410</v>
+        <v>514</v>
       </c>
       <c r="B40" s="18" t="s">
-        <v>411</v>
+        <v>392</v>
       </c>
       <c r="C40" s="17" t="s">
         <v>118</v>
@@ -7289,12 +7925,12 @@
       </c>
       <c r="G40" s="30"/>
     </row>
-    <row r="41" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" ht="75" x14ac:dyDescent="0.2">
       <c r="A41" s="17" t="s">
-        <v>412</v>
+        <v>515</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>413</v>
+        <v>393</v>
       </c>
       <c r="C41" s="17" t="s">
         <v>118</v>
@@ -7310,12 +7946,12 @@
       </c>
       <c r="G41" s="30"/>
     </row>
-    <row r="42" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" ht="60" x14ac:dyDescent="0.2">
       <c r="A42" s="17" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B42" s="18" t="s">
-        <v>414</v>
+        <v>394</v>
       </c>
       <c r="C42" s="17" t="s">
         <v>118</v>
@@ -7331,12 +7967,12 @@
         <v>331</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A43" s="17" t="s">
-        <v>416</v>
+        <v>396</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>415</v>
+        <v>395</v>
       </c>
       <c r="C43" s="49" t="s">
         <v>122</v>
@@ -7346,12 +7982,12 @@
       <c r="F43" s="11"/>
       <c r="G43" s="11"/>
     </row>
-    <row r="44" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A44" s="17" t="s">
-        <v>417</v>
+        <v>516</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>418</v>
+        <v>397</v>
       </c>
       <c r="C44" s="17" t="s">
         <v>118</v>
@@ -7367,12 +8003,12 @@
       </c>
       <c r="G44" s="30"/>
     </row>
-    <row r="45" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" ht="90" x14ac:dyDescent="0.2">
       <c r="A45" s="17" t="s">
-        <v>419</v>
+        <v>398</v>
       </c>
       <c r="B45" s="18" t="s">
-        <v>420</v>
+        <v>399</v>
       </c>
       <c r="C45" s="17" t="s">
         <v>118</v>
@@ -7388,12 +8024,12 @@
       </c>
       <c r="G45" s="30"/>
     </row>
-    <row r="46" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A46" s="17" t="s">
-        <v>421</v>
+        <v>400</v>
       </c>
       <c r="B46" s="18" t="s">
-        <v>423</v>
+        <v>402</v>
       </c>
       <c r="C46" s="17" t="s">
         <v>118</v>
@@ -7409,12 +8045,12 @@
       </c>
       <c r="G46" s="30"/>
     </row>
-    <row r="47" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A47" s="17" t="s">
-        <v>422</v>
+        <v>401</v>
       </c>
       <c r="B47" s="18" t="s">
-        <v>424</v>
+        <v>403</v>
       </c>
       <c r="C47" s="17" t="s">
         <v>118</v>
@@ -7430,12 +8066,12 @@
       </c>
       <c r="G47" s="30"/>
     </row>
-    <row r="48" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A48" s="17" t="s">
-        <v>426</v>
+        <v>517</v>
       </c>
       <c r="B48" s="18" t="s">
-        <v>425</v>
+        <v>404</v>
       </c>
       <c r="C48" s="17" t="s">
         <v>118</v>
@@ -7451,12 +8087,12 @@
       </c>
       <c r="G48" s="30"/>
     </row>
-    <row r="49" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" ht="90" x14ac:dyDescent="0.2">
       <c r="A49" s="17" t="s">
-        <v>428</v>
+        <v>518</v>
       </c>
       <c r="B49" s="18" t="s">
-        <v>427</v>
+        <v>405</v>
       </c>
       <c r="C49" s="17" t="s">
         <v>118</v>
@@ -7472,12 +8108,12 @@
       </c>
       <c r="G49" s="30"/>
     </row>
-    <row r="50" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A50" s="17" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B50" s="18" t="s">
-        <v>433</v>
+        <v>410</v>
       </c>
       <c r="C50" s="49" t="s">
         <v>123</v>
@@ -7487,12 +8123,12 @@
       <c r="F50" s="11"/>
       <c r="G50" s="11"/>
     </row>
-    <row r="51" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A51" s="31" t="s">
+        <v>377</v>
+      </c>
+      <c r="B51" s="32" t="s">
         <v>378</v>
-      </c>
-      <c r="B51" s="32" t="s">
-        <v>379</v>
       </c>
       <c r="C51" s="33" t="s">
         <v>118</v>
@@ -7508,12 +8144,12 @@
       </c>
       <c r="G51" s="30"/>
     </row>
-    <row r="52" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A52" s="31" t="s">
+        <v>361</v>
+      </c>
+      <c r="B52" s="32" t="s">
         <v>362</v>
-      </c>
-      <c r="B52" s="32" t="s">
-        <v>363</v>
       </c>
       <c r="C52" s="33" t="s">
         <v>118</v>
@@ -7529,12 +8165,12 @@
       </c>
       <c r="G52" s="30"/>
     </row>
-    <row r="53" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A53" s="31" t="s">
+        <v>361</v>
+      </c>
+      <c r="B53" s="32" t="s">
         <v>362</v>
-      </c>
-      <c r="B53" s="32" t="s">
-        <v>363</v>
       </c>
       <c r="C53" s="33" t="s">
         <v>118</v>
@@ -7550,12 +8186,12 @@
       </c>
       <c r="G53" s="30"/>
     </row>
-    <row r="54" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A54" s="31" t="s">
-        <v>463</v>
+        <v>440</v>
       </c>
       <c r="B54" s="32" t="s">
-        <v>464</v>
+        <v>441</v>
       </c>
       <c r="C54" s="33" t="s">
         <v>118</v>
@@ -7573,12 +8209,12 @@
         <v>340</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" ht="75" x14ac:dyDescent="0.2">
       <c r="A55" s="31" t="s">
+        <v>361</v>
+      </c>
+      <c r="B55" s="32" t="s">
         <v>362</v>
-      </c>
-      <c r="B55" s="32" t="s">
-        <v>363</v>
       </c>
       <c r="C55" s="33" t="s">
         <v>118</v>
@@ -7594,12 +8230,12 @@
       </c>
       <c r="G55" s="30"/>
     </row>
-    <row r="56" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" ht="90" x14ac:dyDescent="0.2">
       <c r="A56" s="31" t="s">
-        <v>429</v>
+        <v>406</v>
       </c>
       <c r="B56" s="32" t="s">
-        <v>430</v>
+        <v>407</v>
       </c>
       <c r="C56" s="33" t="s">
         <v>118</v>
@@ -7615,12 +8251,12 @@
       </c>
       <c r="G56" s="30"/>
     </row>
-    <row r="57" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A57" s="31" t="s">
-        <v>431</v>
+        <v>408</v>
       </c>
       <c r="B57" s="32" t="s">
-        <v>432</v>
+        <v>409</v>
       </c>
       <c r="C57" s="33" t="s">
         <v>118</v>
@@ -7636,12 +8272,12 @@
       </c>
       <c r="G57" s="30"/>
     </row>
-    <row r="58" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" ht="60" x14ac:dyDescent="0.2">
       <c r="A58" s="31" t="s">
-        <v>431</v>
+        <v>408</v>
       </c>
       <c r="B58" s="32" t="s">
-        <v>432</v>
+        <v>409</v>
       </c>
       <c r="C58" s="33" t="s">
         <v>118</v>
@@ -7657,12 +8293,12 @@
       </c>
       <c r="G58" s="30"/>
     </row>
-    <row r="59" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A59" s="17" t="s">
-        <v>431</v>
+        <v>408</v>
       </c>
       <c r="B59" s="18" t="s">
-        <v>432</v>
+        <v>409</v>
       </c>
       <c r="C59" s="49" t="s">
         <v>124</v>
@@ -7672,12 +8308,12 @@
       <c r="F59" s="11"/>
       <c r="G59" s="11"/>
     </row>
-    <row r="60" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" ht="60" x14ac:dyDescent="0.2">
       <c r="A60" s="31" t="s">
-        <v>431</v>
+        <v>408</v>
       </c>
       <c r="B60" s="32" t="s">
-        <v>432</v>
+        <v>409</v>
       </c>
       <c r="C60" s="17" t="s">
         <v>118</v>
@@ -7693,12 +8329,12 @@
       </c>
       <c r="G60" s="28"/>
     </row>
-    <row r="61" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" ht="60" x14ac:dyDescent="0.2">
       <c r="A61" s="31" t="s">
-        <v>466</v>
+        <v>443</v>
       </c>
       <c r="B61" s="32" t="s">
-        <v>465</v>
+        <v>442</v>
       </c>
       <c r="C61" s="17" t="s">
         <v>118</v>
@@ -7714,12 +8350,12 @@
       </c>
       <c r="G61" s="28"/>
     </row>
-    <row r="62" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" ht="105" x14ac:dyDescent="0.2">
       <c r="A62" s="31" t="s">
-        <v>463</v>
+        <v>440</v>
       </c>
       <c r="B62" s="32" t="s">
-        <v>464</v>
+        <v>441</v>
       </c>
       <c r="C62" s="17" t="s">
         <v>118</v>
@@ -7737,12 +8373,12 @@
         <v>341</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" ht="75" x14ac:dyDescent="0.2">
       <c r="A63" s="31" t="s">
-        <v>467</v>
+        <v>444</v>
       </c>
       <c r="B63" s="32" t="s">
-        <v>468</v>
+        <v>445</v>
       </c>
       <c r="C63" s="17" t="s">
         <v>118</v>
@@ -7758,12 +8394,12 @@
       </c>
       <c r="G63" s="28"/>
     </row>
-    <row r="64" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A64" s="31" t="s">
-        <v>431</v>
+        <v>408</v>
       </c>
       <c r="B64" s="32" t="s">
-        <v>432</v>
+        <v>409</v>
       </c>
       <c r="C64" s="17" t="s">
         <v>118</v>
@@ -7779,12 +8415,12 @@
         <v>331</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A65" s="31" t="s">
-        <v>406</v>
+        <v>389</v>
       </c>
       <c r="B65" s="32" t="s">
-        <v>407</v>
+        <v>390</v>
       </c>
       <c r="C65" s="17" t="s">
         <v>118</v>
@@ -7800,12 +8436,12 @@
       </c>
       <c r="G65" s="28"/>
     </row>
-    <row r="66" spans="1:8" ht="18" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A66" s="17" t="s">
-        <v>429</v>
+        <v>406</v>
       </c>
       <c r="B66" s="18" t="s">
-        <v>430</v>
+        <v>407</v>
       </c>
       <c r="C66" s="49" t="s">
         <v>125</v>
@@ -7815,12 +8451,12 @@
       <c r="F66" s="11"/>
       <c r="G66" s="11"/>
     </row>
-    <row r="67" spans="1:8" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A67" s="36" t="s">
-        <v>471</v>
+        <v>519</v>
       </c>
       <c r="B67" s="37" t="s">
-        <v>457</v>
+        <v>434</v>
       </c>
       <c r="C67" s="36" t="s">
         <v>118</v>
@@ -7837,12 +8473,12 @@
       <c r="G67" s="41"/>
       <c r="H67" s="10"/>
     </row>
-    <row r="68" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A68" s="31" t="s">
-        <v>470</v>
+        <v>447</v>
       </c>
       <c r="B68" s="32" t="s">
-        <v>469</v>
+        <v>446</v>
       </c>
       <c r="C68" s="17" t="s">
         <v>118</v>
@@ -7858,12 +8494,12 @@
       </c>
       <c r="G68" s="28"/>
     </row>
-    <row r="69" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A69" s="31" t="s">
+        <v>371</v>
+      </c>
+      <c r="B69" s="32" t="s">
         <v>372</v>
-      </c>
-      <c r="B69" s="32" t="s">
-        <v>373</v>
       </c>
       <c r="C69" s="17" t="s">
         <v>118</v>
@@ -7879,12 +8515,12 @@
       </c>
       <c r="G69" s="28"/>
     </row>
-    <row r="70" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A70" s="31" t="s">
-        <v>429</v>
+        <v>406</v>
       </c>
       <c r="B70" s="32" t="s">
-        <v>430</v>
+        <v>407</v>
       </c>
       <c r="C70" s="17" t="s">
         <v>118</v>
@@ -7900,12 +8536,12 @@
       </c>
       <c r="G70" s="28"/>
     </row>
-    <row r="71" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A71" s="31" t="s">
+        <v>361</v>
+      </c>
+      <c r="B71" s="32" t="s">
         <v>362</v>
-      </c>
-      <c r="B71" s="32" t="s">
-        <v>363</v>
       </c>
       <c r="C71" s="17" t="s">
         <v>118</v>
@@ -7921,12 +8557,12 @@
         <v>331</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A72" s="31" t="s">
-        <v>472</v>
+        <v>448</v>
       </c>
       <c r="B72" s="32" t="s">
-        <v>473</v>
+        <v>449</v>
       </c>
       <c r="C72" s="17" t="s">
         <v>118</v>
@@ -7942,12 +8578,12 @@
         <v>331</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="18" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A73" s="17" t="s">
-        <v>434</v>
+        <v>411</v>
       </c>
       <c r="B73" s="18" t="s">
-        <v>435</v>
+        <v>412</v>
       </c>
       <c r="C73" s="49" t="s">
         <v>126</v>
@@ -7957,12 +8593,12 @@
       <c r="F73" s="11"/>
       <c r="G73" s="11"/>
     </row>
-    <row r="74" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:8" ht="135" x14ac:dyDescent="0.2">
       <c r="A74" s="31" t="s">
-        <v>434</v>
+        <v>411</v>
       </c>
       <c r="B74" s="32" t="s">
-        <v>435</v>
+        <v>412</v>
       </c>
       <c r="C74" s="17" t="s">
         <v>118</v>
@@ -7978,12 +8614,12 @@
       </c>
       <c r="G74" s="30"/>
     </row>
-    <row r="75" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A75" s="31" t="s">
-        <v>475</v>
+        <v>520</v>
       </c>
       <c r="B75" s="32" t="s">
-        <v>474</v>
+        <v>450</v>
       </c>
       <c r="C75" s="17" t="s">
         <v>118</v>
@@ -7999,12 +8635,12 @@
       </c>
       <c r="G75" s="30"/>
     </row>
-    <row r="76" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A76" s="31" t="s">
-        <v>434</v>
+        <v>411</v>
       </c>
       <c r="B76" s="32" t="s">
-        <v>435</v>
+        <v>412</v>
       </c>
       <c r="C76" s="17" t="s">
         <v>118</v>
@@ -8020,12 +8656,12 @@
       </c>
       <c r="G76" s="30"/>
     </row>
-    <row r="77" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A77" s="31" t="s">
-        <v>477</v>
+        <v>452</v>
       </c>
       <c r="B77" s="32" t="s">
-        <v>476</v>
+        <v>451</v>
       </c>
       <c r="C77" s="17" t="s">
         <v>118</v>
@@ -8041,12 +8677,12 @@
       </c>
       <c r="G77" s="30"/>
     </row>
-    <row r="78" spans="1:8" ht="18" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A78" s="17" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B78" s="18" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C78" s="49" t="s">
         <v>127</v>
@@ -8056,12 +8692,12 @@
       <c r="F78" s="11"/>
       <c r="G78" s="11"/>
     </row>
-    <row r="79" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:8" ht="90" x14ac:dyDescent="0.2">
       <c r="A79" s="31" t="s">
-        <v>392</v>
+        <v>502</v>
       </c>
       <c r="B79" s="32" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C79" s="17" t="s">
         <v>119</v>
@@ -8077,12 +8713,12 @@
       </c>
       <c r="G79" s="28"/>
     </row>
-    <row r="80" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:8" ht="75" x14ac:dyDescent="0.2">
       <c r="A80" s="31" t="s">
-        <v>481</v>
+        <v>521</v>
       </c>
       <c r="B80" s="32" t="s">
-        <v>480</v>
+        <v>455</v>
       </c>
       <c r="C80" s="17" t="s">
         <v>119</v>
@@ -8098,12 +8734,12 @@
       </c>
       <c r="G80" s="28"/>
     </row>
-    <row r="81" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A81" s="31" t="s">
-        <v>393</v>
+        <v>503</v>
       </c>
       <c r="B81" s="32" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C81" s="17" t="s">
         <v>119</v>
@@ -8119,12 +8755,12 @@
       </c>
       <c r="G81" s="28"/>
     </row>
-    <row r="82" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="31" t="s">
-        <v>478</v>
+        <v>453</v>
       </c>
       <c r="B82" s="32" t="s">
-        <v>479</v>
+        <v>454</v>
       </c>
       <c r="C82" s="17" t="s">
         <v>119</v>
@@ -8140,12 +8776,12 @@
       </c>
       <c r="G82" s="28"/>
     </row>
-    <row r="83" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="31" t="s">
+        <v>377</v>
+      </c>
+      <c r="B83" s="32" t="s">
         <v>378</v>
-      </c>
-      <c r="B83" s="32" t="s">
-        <v>379</v>
       </c>
       <c r="C83" s="17" t="s">
         <v>119</v>
@@ -8161,12 +8797,12 @@
       </c>
       <c r="G83" s="28"/>
     </row>
-    <row r="84" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" ht="60" x14ac:dyDescent="0.2">
       <c r="A84" s="31" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B84" s="32" t="s">
-        <v>414</v>
+        <v>394</v>
       </c>
       <c r="C84" s="17" t="s">
         <v>119</v>
@@ -8182,12 +8818,12 @@
         <v>331</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A85" s="31" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B85" s="32" t="s">
-        <v>414</v>
+        <v>394</v>
       </c>
       <c r="C85" s="17" t="s">
         <v>119</v>
@@ -8203,12 +8839,12 @@
       </c>
       <c r="G85" s="28"/>
     </row>
-    <row r="86" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A86" s="17" t="s">
-        <v>429</v>
+        <v>406</v>
       </c>
       <c r="B86" s="18" t="s">
-        <v>430</v>
+        <v>407</v>
       </c>
       <c r="C86" s="49" t="s">
         <v>128</v>
@@ -8218,12 +8854,12 @@
       <c r="F86" s="11"/>
       <c r="G86" s="11"/>
     </row>
-    <row r="87" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" ht="105" x14ac:dyDescent="0.2">
       <c r="A87" s="31" t="s">
-        <v>512</v>
+        <v>522</v>
       </c>
       <c r="B87" s="32" t="s">
-        <v>511</v>
+        <v>481</v>
       </c>
       <c r="C87" s="17" t="s">
         <v>119</v>
@@ -8239,12 +8875,12 @@
       </c>
       <c r="G87" s="28"/>
     </row>
-    <row r="88" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" ht="90" x14ac:dyDescent="0.2">
       <c r="A88" s="31" t="s">
-        <v>428</v>
+        <v>518</v>
       </c>
       <c r="B88" s="32" t="s">
-        <v>427</v>
+        <v>405</v>
       </c>
       <c r="C88" s="17" t="s">
         <v>119</v>
@@ -8260,12 +8896,12 @@
       </c>
       <c r="G88" s="28"/>
     </row>
-    <row r="89" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" ht="60" x14ac:dyDescent="0.2">
       <c r="A89" s="31" t="s">
-        <v>514</v>
+        <v>523</v>
       </c>
       <c r="B89" s="32" t="s">
-        <v>513</v>
+        <v>482</v>
       </c>
       <c r="C89" s="17" t="s">
         <v>119</v>
@@ -8281,12 +8917,12 @@
       </c>
       <c r="G89" s="28"/>
     </row>
-    <row r="90" spans="1:7" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" ht="105" x14ac:dyDescent="0.2">
       <c r="A90" s="31" t="s">
-        <v>463</v>
+        <v>440</v>
       </c>
       <c r="B90" s="32" t="s">
-        <v>464</v>
+        <v>441</v>
       </c>
       <c r="C90" s="17" t="s">
         <v>119</v>
@@ -8302,12 +8938,12 @@
       </c>
       <c r="G90" s="28"/>
     </row>
-    <row r="91" spans="1:7" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" ht="105" x14ac:dyDescent="0.2">
       <c r="A91" s="31" t="s">
-        <v>516</v>
+        <v>524</v>
       </c>
       <c r="B91" s="32" t="s">
-        <v>515</v>
+        <v>483</v>
       </c>
       <c r="C91" s="17" t="s">
         <v>119</v>
@@ -8323,12 +8959,12 @@
       </c>
       <c r="G91" s="28"/>
     </row>
-    <row r="92" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A92" s="48" t="s">
-        <v>409</v>
+        <v>513</v>
       </c>
       <c r="B92" s="32" t="s">
-        <v>408</v>
+        <v>391</v>
       </c>
       <c r="C92" s="17" t="s">
         <v>119</v>
@@ -8344,12 +8980,12 @@
       </c>
       <c r="G92" s="28"/>
     </row>
-    <row r="93" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" ht="75" x14ac:dyDescent="0.2">
       <c r="A93" s="31" t="s">
-        <v>518</v>
+        <v>525</v>
       </c>
       <c r="B93" s="32" t="s">
-        <v>517</v>
+        <v>484</v>
       </c>
       <c r="C93" s="17" t="s">
         <v>119</v>
@@ -8365,12 +9001,12 @@
         <v>331</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" ht="60" x14ac:dyDescent="0.2">
       <c r="A94" s="31" t="s">
-        <v>463</v>
+        <v>440</v>
       </c>
       <c r="B94" s="32" t="s">
-        <v>464</v>
+        <v>441</v>
       </c>
       <c r="C94" s="17" t="s">
         <v>119</v>
@@ -8386,12 +9022,12 @@
         <v>331</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A95" s="31" t="s">
-        <v>520</v>
+        <v>526</v>
       </c>
       <c r="B95" s="32" t="s">
-        <v>519</v>
+        <v>485</v>
       </c>
       <c r="C95" s="17" t="s">
         <v>119</v>
@@ -8407,12 +9043,12 @@
       </c>
       <c r="G95" s="28"/>
     </row>
-    <row r="96" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" ht="75" x14ac:dyDescent="0.2">
       <c r="A96" s="31" t="s">
-        <v>522</v>
+        <v>527</v>
       </c>
       <c r="B96" s="32" t="s">
-        <v>521</v>
+        <v>486</v>
       </c>
       <c r="C96" s="17" t="s">
         <v>119</v>
@@ -8428,12 +9064,12 @@
         <v>331</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="24" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A97" s="17" t="s">
-        <v>448</v>
+        <v>425</v>
       </c>
       <c r="B97" s="18" t="s">
-        <v>449</v>
+        <v>426</v>
       </c>
       <c r="C97" s="49" t="s">
         <v>129</v>
@@ -8443,12 +9079,12 @@
       <c r="F97" s="11"/>
       <c r="G97" s="11"/>
     </row>
-    <row r="98" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A98" s="31" t="s">
-        <v>524</v>
+        <v>488</v>
       </c>
       <c r="B98" s="32" t="s">
-        <v>523</v>
+        <v>487</v>
       </c>
       <c r="C98" s="17" t="s">
         <v>119</v>
@@ -8464,12 +9100,12 @@
       </c>
       <c r="G98" s="28"/>
     </row>
-    <row r="99" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A99" s="31" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
       <c r="B99" s="32" t="s">
-        <v>525</v>
+        <v>489</v>
       </c>
       <c r="C99" s="17" t="s">
         <v>119</v>
@@ -8485,12 +9121,12 @@
       </c>
       <c r="G99" s="28"/>
     </row>
-    <row r="100" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A100" s="31" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B100" s="32" t="s">
-        <v>527</v>
+        <v>490</v>
       </c>
       <c r="C100" s="17" t="s">
         <v>119</v>
@@ -8506,12 +9142,12 @@
         <v>331</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:8" ht="75" x14ac:dyDescent="0.2">
       <c r="A101" s="31" t="s">
         <v>530</v>
       </c>
       <c r="B101" s="32" t="s">
-        <v>529</v>
+        <v>491</v>
       </c>
       <c r="C101" s="17" t="s">
         <v>119</v>
@@ -8527,12 +9163,12 @@
         <v>331</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:8" ht="90" x14ac:dyDescent="0.2">
       <c r="A102" s="31" t="s">
-        <v>531</v>
+        <v>492</v>
       </c>
       <c r="B102" s="32" t="s">
-        <v>532</v>
+        <v>493</v>
       </c>
       <c r="C102" s="17" t="s">
         <v>119</v>
@@ -8548,12 +9184,12 @@
         <v>331</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A103" s="31" t="s">
-        <v>426</v>
+        <v>517</v>
       </c>
       <c r="B103" s="32" t="s">
-        <v>425</v>
+        <v>404</v>
       </c>
       <c r="C103" s="17" t="s">
         <v>119</v>
@@ -8569,12 +9205,12 @@
         <v>331</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A104" s="31" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="B104" s="32" t="s">
-        <v>533</v>
+        <v>494</v>
       </c>
       <c r="C104" s="17" t="s">
         <v>119</v>
@@ -8590,12 +9226,12 @@
         <v>331</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="24" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A105" s="31" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B105" s="32" t="s">
-        <v>527</v>
+        <v>490</v>
       </c>
       <c r="C105" s="17" t="s">
         <v>119</v>
@@ -8611,12 +9247,12 @@
         <v>331</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A106" s="31" t="s">
-        <v>456</v>
+        <v>433</v>
       </c>
       <c r="B106" s="32" t="s">
-        <v>460</v>
+        <v>437</v>
       </c>
       <c r="C106" s="17" t="s">
         <v>119</v>
@@ -8632,12 +9268,12 @@
         <v>331</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="18" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A107" s="17" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B107" s="18" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C107" s="49" t="s">
         <v>134</v>
@@ -8647,12 +9283,12 @@
       <c r="F107" s="11"/>
       <c r="G107" s="11"/>
     </row>
-    <row r="108" spans="1:8" s="8" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:8" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A108" s="36" t="s">
-        <v>450</v>
+        <v>427</v>
       </c>
       <c r="B108" s="42" t="s">
-        <v>458</v>
+        <v>435</v>
       </c>
       <c r="C108" s="36" t="s">
         <v>120</v>
@@ -8668,15 +9304,15 @@
       </c>
       <c r="G108" s="41"/>
       <c r="H108" s="10" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" s="8" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A109" s="36" t="s">
-        <v>452</v>
+        <v>429</v>
       </c>
       <c r="B109" s="42" t="s">
-        <v>459</v>
+        <v>436</v>
       </c>
       <c r="C109" s="36" t="s">
         <v>120</v>
@@ -8693,12 +9329,12 @@
       <c r="G109" s="41"/>
       <c r="H109" s="10"/>
     </row>
-    <row r="110" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A110" s="46" t="s">
-        <v>450</v>
+        <v>427</v>
       </c>
       <c r="B110" s="47" t="s">
-        <v>458</v>
+        <v>435</v>
       </c>
       <c r="C110" s="17" t="s">
         <v>120</v>
@@ -8714,12 +9350,12 @@
       </c>
       <c r="G110" s="28"/>
     </row>
-    <row r="111" spans="1:8" s="8" customFormat="1" ht="72" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:8" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A111" s="36" t="s">
-        <v>456</v>
+        <v>433</v>
       </c>
       <c r="B111" s="42" t="s">
-        <v>460</v>
+        <v>437</v>
       </c>
       <c r="C111" s="36" t="s">
         <v>120</v>
@@ -8736,12 +9372,12 @@
       <c r="G111" s="41"/>
       <c r="H111" s="10"/>
     </row>
-    <row r="112" spans="1:8" s="8" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:8" s="8" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A112" s="36" t="s">
-        <v>453</v>
+        <v>430</v>
       </c>
       <c r="B112" s="42" t="s">
-        <v>461</v>
+        <v>438</v>
       </c>
       <c r="C112" s="36" t="s">
         <v>120</v>
@@ -8758,12 +9394,12 @@
       </c>
       <c r="H112" s="10"/>
     </row>
-    <row r="113" spans="1:8" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:8" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A113" s="36" t="s">
-        <v>406</v>
+        <v>389</v>
       </c>
       <c r="B113" s="42" t="s">
-        <v>407</v>
+        <v>390</v>
       </c>
       <c r="C113" s="36" t="s">
         <v>120</v>
@@ -8780,12 +9416,12 @@
       <c r="G113" s="41"/>
       <c r="H113" s="10"/>
     </row>
-    <row r="114" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A114" s="31" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B114" s="32" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C114" s="17" t="s">
         <v>120</v>
@@ -8801,12 +9437,12 @@
       </c>
       <c r="G114" s="28"/>
     </row>
-    <row r="115" spans="1:8" ht="18" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A115" s="17" t="s">
-        <v>436</v>
+        <v>413</v>
       </c>
       <c r="B115" s="18" t="s">
-        <v>437</v>
+        <v>414</v>
       </c>
       <c r="C115" s="49" t="s">
         <v>133</v>
@@ -8816,12 +9452,12 @@
       <c r="F115" s="11"/>
       <c r="G115" s="11"/>
     </row>
-    <row r="116" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A116" s="31" t="s">
-        <v>500</v>
+        <v>472</v>
       </c>
       <c r="B116" s="32" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C116" s="17" t="s">
         <v>119</v>
@@ -8837,12 +9473,12 @@
       </c>
       <c r="G116" s="28"/>
     </row>
-    <row r="117" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A117" s="31" t="s">
-        <v>491</v>
+        <v>532</v>
       </c>
       <c r="B117" s="32" t="s">
-        <v>490</v>
+        <v>463</v>
       </c>
       <c r="C117" s="17" t="s">
         <v>119</v>
@@ -8858,12 +9494,12 @@
       </c>
       <c r="G117" s="28"/>
     </row>
-    <row r="118" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A118" s="31" t="s">
-        <v>491</v>
+        <v>532</v>
       </c>
       <c r="B118" s="32" t="s">
-        <v>490</v>
+        <v>463</v>
       </c>
       <c r="C118" s="17" t="s">
         <v>119</v>
@@ -8879,12 +9515,12 @@
         <v>331</v>
       </c>
     </row>
-    <row r="119" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A119" s="31" t="s">
+        <v>361</v>
+      </c>
+      <c r="B119" s="32" t="s">
         <v>362</v>
-      </c>
-      <c r="B119" s="32" t="s">
-        <v>363</v>
       </c>
       <c r="C119" s="17" t="s">
         <v>119</v>
@@ -8900,12 +9536,12 @@
         <v>331</v>
       </c>
     </row>
-    <row r="120" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A120" s="31" t="s">
-        <v>502</v>
+        <v>533</v>
       </c>
       <c r="B120" s="32" t="s">
-        <v>501</v>
+        <v>473</v>
       </c>
       <c r="C120" s="17" t="s">
         <v>119</v>
@@ -8921,12 +9557,12 @@
       </c>
       <c r="G120" s="28"/>
     </row>
-    <row r="121" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A121" s="31" t="s">
-        <v>502</v>
+        <v>533</v>
       </c>
       <c r="B121" s="32" t="s">
-        <v>501</v>
+        <v>473</v>
       </c>
       <c r="C121" s="17" t="s">
         <v>119</v>
@@ -8942,12 +9578,12 @@
       </c>
       <c r="G121" s="28"/>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" s="31" t="s">
+        <v>361</v>
+      </c>
+      <c r="B122" s="32" t="s">
         <v>362</v>
-      </c>
-      <c r="B122" s="32" t="s">
-        <v>363</v>
       </c>
       <c r="C122" s="17" t="s">
         <v>119</v>
@@ -8963,12 +9599,12 @@
       </c>
       <c r="G122" s="28"/>
     </row>
-    <row r="123" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A123" s="31" t="s">
+        <v>361</v>
+      </c>
+      <c r="B123" s="32" t="s">
         <v>362</v>
-      </c>
-      <c r="B123" s="32" t="s">
-        <v>363</v>
       </c>
       <c r="C123" s="17" t="s">
         <v>119</v>
@@ -8984,12 +9620,12 @@
       </c>
       <c r="G123" s="28"/>
     </row>
-    <row r="124" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A124" s="46" t="s">
-        <v>450</v>
+        <v>427</v>
       </c>
       <c r="B124" s="47" t="s">
-        <v>458</v>
+        <v>435</v>
       </c>
       <c r="C124" s="17" t="s">
         <v>119</v>
@@ -9005,12 +9641,12 @@
       </c>
       <c r="G124" s="28"/>
     </row>
-    <row r="125" spans="1:8" ht="18" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A125" s="17" t="s">
-        <v>438</v>
+        <v>415</v>
       </c>
       <c r="B125" s="18" t="s">
-        <v>439</v>
+        <v>416</v>
       </c>
       <c r="C125" s="49" t="s">
         <v>70</v>
@@ -9020,12 +9656,12 @@
       <c r="F125" s="11"/>
       <c r="G125" s="11"/>
     </row>
-    <row r="126" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A126" s="31" t="s">
-        <v>495</v>
+        <v>467</v>
       </c>
       <c r="B126" s="32" t="s">
-        <v>494</v>
+        <v>466</v>
       </c>
       <c r="C126" s="17" t="s">
         <v>120</v>
@@ -9041,12 +9677,12 @@
       </c>
       <c r="G126" s="28"/>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" s="31" t="s">
-        <v>495</v>
+        <v>467</v>
       </c>
       <c r="B127" s="32" t="s">
-        <v>494</v>
+        <v>466</v>
       </c>
       <c r="C127" s="17" t="s">
         <v>120</v>
@@ -9062,12 +9698,12 @@
       </c>
       <c r="G127" s="28"/>
     </row>
-    <row r="128" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A128" s="31" t="s">
-        <v>493</v>
+        <v>465</v>
       </c>
       <c r="B128" s="32" t="s">
-        <v>492</v>
+        <v>464</v>
       </c>
       <c r="C128" s="17" t="s">
         <v>120</v>
@@ -9083,12 +9719,12 @@
       </c>
       <c r="G128" s="28"/>
     </row>
-    <row r="129" spans="1:8" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.2">
       <c r="A129" s="36" t="s">
-        <v>455</v>
+        <v>432</v>
       </c>
       <c r="B129" s="42" t="s">
-        <v>462</v>
+        <v>439</v>
       </c>
       <c r="C129" s="36" t="s">
         <v>120</v>
@@ -9105,12 +9741,12 @@
       <c r="G129" s="41"/>
       <c r="H129" s="10"/>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A130" s="31" t="s">
-        <v>496</v>
+        <v>468</v>
       </c>
       <c r="B130" s="32" t="s">
-        <v>497</v>
+        <v>469</v>
       </c>
       <c r="C130" s="17" t="s">
         <v>120</v>
@@ -9126,12 +9762,12 @@
       </c>
       <c r="G130" s="28"/>
     </row>
-    <row r="131" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" ht="90" x14ac:dyDescent="0.2">
       <c r="A131" s="31" t="s">
-        <v>495</v>
+        <v>467</v>
       </c>
       <c r="B131" s="32" t="s">
-        <v>494</v>
+        <v>466</v>
       </c>
       <c r="C131" s="17" t="s">
         <v>120</v>
@@ -9147,12 +9783,12 @@
       </c>
       <c r="G131" s="28"/>
     </row>
-    <row r="132" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A132" s="31" t="s">
-        <v>498</v>
+        <v>470</v>
       </c>
       <c r="B132" s="32" t="s">
-        <v>499</v>
+        <v>471</v>
       </c>
       <c r="C132" s="17" t="s">
         <v>120</v>
@@ -9168,12 +9804,12 @@
       </c>
       <c r="G132" s="28"/>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A133" s="31" t="s">
-        <v>406</v>
+        <v>389</v>
       </c>
       <c r="B133" s="32" t="s">
-        <v>407</v>
+        <v>390</v>
       </c>
       <c r="C133" s="17" t="s">
         <v>120</v>
@@ -9189,12 +9825,12 @@
       </c>
       <c r="G133" s="28"/>
     </row>
-    <row r="134" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A134" s="31" t="s">
-        <v>438</v>
+        <v>415</v>
       </c>
       <c r="B134" s="32" t="s">
-        <v>439</v>
+        <v>416</v>
       </c>
       <c r="C134" s="17" t="s">
         <v>120</v>
@@ -9210,12 +9846,12 @@
       </c>
       <c r="G134" s="28"/>
     </row>
-    <row r="135" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8" ht="75" x14ac:dyDescent="0.2">
       <c r="A135" s="31" t="s">
-        <v>402</v>
+        <v>386</v>
       </c>
       <c r="B135" s="32" t="s">
-        <v>403</v>
+        <v>387</v>
       </c>
       <c r="C135" s="17" t="s">
         <v>120</v>
@@ -9231,12 +9867,12 @@
         <v>331</v>
       </c>
     </row>
-    <row r="136" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A136" s="31" t="s">
-        <v>409</v>
+        <v>513</v>
       </c>
       <c r="B136" s="32" t="s">
-        <v>408</v>
+        <v>391</v>
       </c>
       <c r="C136" s="17" t="s">
         <v>120</v>
@@ -9252,12 +9888,12 @@
       </c>
       <c r="G136" s="28"/>
     </row>
-    <row r="137" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A137" s="31" t="s">
-        <v>505</v>
+        <v>475</v>
       </c>
       <c r="B137" s="32" t="s">
-        <v>506</v>
+        <v>476</v>
       </c>
       <c r="C137" s="17" t="s">
         <v>120</v>
@@ -9273,12 +9909,12 @@
       </c>
       <c r="G137" s="28"/>
     </row>
-    <row r="138" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A138" s="31" t="s">
-        <v>452</v>
+        <v>429</v>
       </c>
       <c r="B138" s="32" t="s">
-        <v>459</v>
+        <v>436</v>
       </c>
       <c r="C138" s="17" t="s">
         <v>120</v>
@@ -9294,12 +9930,12 @@
       </c>
       <c r="G138" s="28"/>
     </row>
-    <row r="139" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A139" s="31" t="s">
-        <v>453</v>
+        <v>430</v>
       </c>
       <c r="B139" s="32" t="s">
-        <v>461</v>
+        <v>438</v>
       </c>
       <c r="C139" s="17" t="s">
         <v>120</v>
@@ -9315,12 +9951,12 @@
       </c>
       <c r="G139" s="28"/>
     </row>
-    <row r="140" spans="1:8" ht="24" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A140" s="17" t="s">
-        <v>441</v>
+        <v>418</v>
       </c>
       <c r="B140" s="18" t="s">
-        <v>440</v>
+        <v>417</v>
       </c>
       <c r="C140" s="49" t="s">
         <v>130</v>
@@ -9330,12 +9966,12 @@
       <c r="F140" s="11"/>
       <c r="G140" s="11"/>
     </row>
-    <row r="141" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A141" s="31" t="s">
-        <v>510</v>
+        <v>480</v>
       </c>
       <c r="B141" s="32" t="s">
-        <v>509</v>
+        <v>479</v>
       </c>
       <c r="C141" s="17" t="s">
         <v>120</v>
@@ -9351,12 +9987,12 @@
       </c>
       <c r="G141" s="28"/>
     </row>
-    <row r="142" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A142" s="31" t="s">
-        <v>510</v>
+        <v>480</v>
       </c>
       <c r="B142" s="32" t="s">
-        <v>509</v>
+        <v>479</v>
       </c>
       <c r="C142" s="17" t="s">
         <v>120</v>
@@ -9372,12 +10008,12 @@
       </c>
       <c r="G142" s="28"/>
     </row>
-    <row r="143" spans="1:8" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:8" ht="75" x14ac:dyDescent="0.2">
       <c r="A143" s="31" t="s">
-        <v>510</v>
+        <v>480</v>
       </c>
       <c r="B143" s="32" t="s">
-        <v>509</v>
+        <v>479</v>
       </c>
       <c r="C143" s="17" t="s">
         <v>120</v>
@@ -9393,12 +10029,12 @@
       </c>
       <c r="G143" s="28"/>
     </row>
-    <row r="144" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A144" s="31" t="s">
-        <v>510</v>
+        <v>480</v>
       </c>
       <c r="B144" s="32" t="s">
-        <v>509</v>
+        <v>479</v>
       </c>
       <c r="C144" s="17" t="s">
         <v>120</v>
@@ -9414,12 +10050,12 @@
       </c>
       <c r="G144" s="28"/>
     </row>
-    <row r="145" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:8" ht="60" x14ac:dyDescent="0.2">
       <c r="A145" s="31" t="s">
-        <v>510</v>
+        <v>480</v>
       </c>
       <c r="B145" s="32" t="s">
-        <v>509</v>
+        <v>479</v>
       </c>
       <c r="C145" s="17" t="s">
         <v>120</v>
@@ -9435,12 +10071,12 @@
         <v>331</v>
       </c>
     </row>
-    <row r="146" spans="1:8" ht="24" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:8" ht="24" x14ac:dyDescent="0.2">
       <c r="A146" s="17" t="s">
-        <v>442</v>
+        <v>419</v>
       </c>
       <c r="B146" s="18" t="s">
-        <v>443</v>
+        <v>420</v>
       </c>
       <c r="C146" s="49" t="s">
         <v>131</v>
@@ -9450,12 +10086,12 @@
       <c r="F146" s="11"/>
       <c r="G146" s="11"/>
     </row>
-    <row r="147" spans="1:8" s="8" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:8" s="8" customFormat="1" ht="60" x14ac:dyDescent="0.2">
       <c r="A147" s="36" t="s">
+        <v>377</v>
+      </c>
+      <c r="B147" s="42" t="s">
         <v>378</v>
-      </c>
-      <c r="B147" s="42" t="s">
-        <v>379</v>
       </c>
       <c r="C147" s="36" t="s">
         <v>120</v>
@@ -9471,15 +10107,15 @@
       </c>
       <c r="G147" s="41"/>
       <c r="H147" s="10" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="148" spans="1:8" ht="129.6" x14ac:dyDescent="0.3">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" ht="120" x14ac:dyDescent="0.2">
       <c r="A148" s="31" t="s">
-        <v>472</v>
+        <v>448</v>
       </c>
       <c r="B148" s="32" t="s">
-        <v>473</v>
+        <v>449</v>
       </c>
       <c r="C148" s="17" t="s">
         <v>120</v>
@@ -9497,12 +10133,12 @@
         <v>342</v>
       </c>
     </row>
-    <row r="149" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A149" s="31" t="s">
-        <v>472</v>
+        <v>448</v>
       </c>
       <c r="B149" s="32" t="s">
-        <v>473</v>
+        <v>449</v>
       </c>
       <c r="C149" s="17" t="s">
         <v>120</v>
@@ -9518,12 +10154,12 @@
       </c>
       <c r="G149" s="28"/>
     </row>
-    <row r="150" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:8" ht="75" x14ac:dyDescent="0.2">
       <c r="A150" s="31" t="s">
+        <v>371</v>
+      </c>
+      <c r="B150" s="32" t="s">
         <v>372</v>
-      </c>
-      <c r="B150" s="32" t="s">
-        <v>373</v>
       </c>
       <c r="C150" s="17" t="s">
         <v>120</v>
@@ -9539,12 +10175,12 @@
       </c>
       <c r="G150" s="28"/>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A151" s="31" t="s">
-        <v>508</v>
+        <v>478</v>
       </c>
       <c r="B151" s="32" t="s">
-        <v>507</v>
+        <v>477</v>
       </c>
       <c r="C151" s="17" t="s">
         <v>120</v>
@@ -9560,12 +10196,12 @@
       </c>
       <c r="G151" s="28"/>
     </row>
-    <row r="152" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A152" s="31" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B152" s="32" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="C152" s="17" t="s">
         <v>120</v>
@@ -9581,12 +10217,12 @@
       </c>
       <c r="G152" s="28"/>
     </row>
-    <row r="153" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A153" s="31" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B153" s="32" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C153" s="17" t="s">
         <v>120</v>
@@ -9602,12 +10238,12 @@
       </c>
       <c r="G153" s="28"/>
     </row>
-    <row r="154" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A154" s="31" t="s">
-        <v>510</v>
+        <v>480</v>
       </c>
       <c r="B154" s="32" t="s">
-        <v>509</v>
+        <v>479</v>
       </c>
       <c r="C154" s="17" t="s">
         <v>120</v>
@@ -9623,12 +10259,12 @@
       </c>
       <c r="G154" s="28"/>
     </row>
-    <row r="155" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A155" s="31" t="s">
+        <v>361</v>
+      </c>
+      <c r="B155" s="32" t="s">
         <v>362</v>
-      </c>
-      <c r="B155" s="32" t="s">
-        <v>363</v>
       </c>
       <c r="C155" s="17" t="s">
         <v>120</v>
@@ -9644,12 +10280,12 @@
       </c>
       <c r="G155" s="28"/>
     </row>
-    <row r="156" spans="1:8" ht="18" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:8" ht="19" x14ac:dyDescent="0.2">
       <c r="A156" s="17" t="s">
-        <v>445</v>
+        <v>422</v>
       </c>
       <c r="B156" s="18" t="s">
-        <v>444</v>
+        <v>421</v>
       </c>
       <c r="C156" s="49" t="s">
         <v>132</v>
@@ -9659,12 +10295,12 @@
       <c r="F156" s="11"/>
       <c r="G156" s="11"/>
     </row>
-    <row r="157" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:8" ht="45" x14ac:dyDescent="0.2">
       <c r="A157" s="31" t="s">
-        <v>445</v>
+        <v>422</v>
       </c>
       <c r="B157" s="32" t="s">
-        <v>444</v>
+        <v>421</v>
       </c>
       <c r="C157" s="17" t="s">
         <v>120</v>
@@ -9680,12 +10316,12 @@
       </c>
       <c r="G157" s="28"/>
     </row>
-    <row r="158" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A158" s="31" t="s">
-        <v>486</v>
+        <v>459</v>
       </c>
       <c r="B158" s="32" t="s">
-        <v>487</v>
+        <v>460</v>
       </c>
       <c r="C158" s="17" t="s">
         <v>120</v>
@@ -9701,12 +10337,12 @@
       </c>
       <c r="G158" s="28"/>
     </row>
-    <row r="159" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A159" s="31" t="s">
-        <v>486</v>
+        <v>459</v>
       </c>
       <c r="B159" s="32" t="s">
-        <v>487</v>
+        <v>460</v>
       </c>
       <c r="C159" s="17" t="s">
         <v>120</v>
@@ -9722,12 +10358,12 @@
       </c>
       <c r="G159" s="28"/>
     </row>
-    <row r="160" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:8" ht="90" x14ac:dyDescent="0.2">
       <c r="A160" s="31" t="s">
-        <v>488</v>
+        <v>461</v>
       </c>
       <c r="B160" s="32" t="s">
-        <v>489</v>
+        <v>462</v>
       </c>
       <c r="C160" s="17" t="s">
         <v>120</v>
@@ -9743,12 +10379,12 @@
       </c>
       <c r="G160" s="28"/>
     </row>
-    <row r="161" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A161" s="31" t="s">
-        <v>488</v>
+        <v>461</v>
       </c>
       <c r="B161" s="32" t="s">
-        <v>489</v>
+        <v>462</v>
       </c>
       <c r="C161" s="17" t="s">
         <v>120</v>
@@ -9764,12 +10400,12 @@
       </c>
       <c r="G161" s="28"/>
     </row>
-    <row r="162" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A162" s="31" t="s">
-        <v>485</v>
+        <v>458</v>
       </c>
       <c r="B162" s="32" t="s">
-        <v>484</v>
+        <v>457</v>
       </c>
       <c r="C162" s="17" t="s">
         <v>120</v>
@@ -9785,12 +10421,12 @@
       </c>
       <c r="G162" s="28"/>
     </row>
-    <row r="163" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A163" s="31" t="s">
-        <v>485</v>
+        <v>458</v>
       </c>
       <c r="B163" s="32" t="s">
-        <v>484</v>
+        <v>457</v>
       </c>
       <c r="C163" s="17" t="s">
         <v>120</v>
@@ -9806,12 +10442,12 @@
       </c>
       <c r="G163" s="28"/>
     </row>
-    <row r="164" spans="1:7" ht="18" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:7" ht="19" x14ac:dyDescent="0.2">
       <c r="A164" s="17" t="s">
-        <v>446</v>
+        <v>423</v>
       </c>
       <c r="B164" s="18" t="s">
-        <v>447</v>
+        <v>424</v>
       </c>
       <c r="C164" s="49" t="s">
         <v>91</v>
@@ -9821,12 +10457,12 @@
       <c r="F164" s="11"/>
       <c r="G164" s="11"/>
     </row>
-    <row r="165" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:7" ht="75" x14ac:dyDescent="0.2">
       <c r="A165" s="31" t="s">
-        <v>446</v>
+        <v>423</v>
       </c>
       <c r="B165" s="32" t="s">
-        <v>447</v>
+        <v>424</v>
       </c>
       <c r="C165" s="17" t="s">
         <v>120</v>
@@ -9842,12 +10478,12 @@
       </c>
       <c r="G165" s="28"/>
     </row>
-    <row r="166" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A166" s="31" t="s">
-        <v>446</v>
+        <v>423</v>
       </c>
       <c r="B166" s="32" t="s">
-        <v>447</v>
+        <v>424</v>
       </c>
       <c r="C166" s="17" t="s">
         <v>120</v>
@@ -9863,12 +10499,12 @@
       </c>
       <c r="G166" s="28"/>
     </row>
-    <row r="167" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:7" ht="30" x14ac:dyDescent="0.2">
       <c r="A167" s="31" t="s">
-        <v>483</v>
+        <v>534</v>
       </c>
       <c r="B167" s="32" t="s">
-        <v>482</v>
+        <v>456</v>
       </c>
       <c r="C167" s="17" t="s">
         <v>120</v>
@@ -9884,12 +10520,12 @@
       </c>
       <c r="G167" s="28"/>
     </row>
-    <row r="168" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:7" ht="60" x14ac:dyDescent="0.2">
       <c r="A168" s="31" t="s">
-        <v>446</v>
+        <v>423</v>
       </c>
       <c r="B168" s="32" t="s">
-        <v>447</v>
+        <v>424</v>
       </c>
       <c r="C168" s="17" t="s">
         <v>120</v>
@@ -9905,12 +10541,12 @@
       </c>
       <c r="G168" s="28"/>
     </row>
-    <row r="169" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:7" ht="75" x14ac:dyDescent="0.2">
       <c r="A169" s="31" t="s">
-        <v>446</v>
+        <v>423</v>
       </c>
       <c r="B169" s="32" t="s">
-        <v>447</v>
+        <v>424</v>
       </c>
       <c r="C169" s="17" t="s">
         <v>120</v>
@@ -9926,12 +10562,12 @@
       </c>
       <c r="G169" s="28"/>
     </row>
-    <row r="170" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A170" s="31" t="s">
+        <v>371</v>
+      </c>
+      <c r="B170" s="32" t="s">
         <v>372</v>
-      </c>
-      <c r="B170" s="32" t="s">
-        <v>373</v>
       </c>
       <c r="C170" s="17" t="s">
         <v>120</v>
@@ -9947,12 +10583,12 @@
       </c>
       <c r="G170" s="28"/>
     </row>
-    <row r="171" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A171" s="31" t="s">
-        <v>483</v>
+        <v>534</v>
       </c>
       <c r="B171" s="32" t="s">
-        <v>482</v>
+        <v>456</v>
       </c>
       <c r="C171" s="17" t="s">
         <v>120</v>
@@ -9968,12 +10604,12 @@
         <v>331</v>
       </c>
     </row>
-    <row r="172" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:7" ht="45" x14ac:dyDescent="0.2">
       <c r="A172" s="31" t="s">
-        <v>446</v>
+        <v>423</v>
       </c>
       <c r="B172" s="32" t="s">
-        <v>447</v>
+        <v>424</v>
       </c>
       <c r="C172" s="17" t="s">
         <v>120</v>
@@ -9992,9 +10628,9 @@
   </sheetData>
   <autoFilter ref="A3:H172"/>
   <customSheetViews>
-    <customSheetView guid="{9FD8CC1C-6420-44A1-A370-C19CD963FBCC}" scale="85" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1">
+    <customSheetView guid="{D2DB1628-96BC-634F-B558-28007DD1D3D1}" scale="85" fitToPage="1" showAutoFilter="1">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="A172" sqref="A172"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup fitToHeight="0" orientation="landscape" r:id="rId1"/>
       <headerFooter>
@@ -10003,11 +10639,31 @@
       </headerFooter>
       <autoFilter ref="A3:H172"/>
     </customSheetView>
-    <customSheetView guid="{166C989B-D112-4FBE-9337-483856443AEC}" scale="85" fitToPage="1" printArea="1" topLeftCell="B1">
-      <pane ySplit="3" topLeftCell="A144" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="H147" sqref="H147"/>
+    <customSheetView guid="{156F6E94-B77C-4218-9566-01A2D0E67E8E}" scale="90" showPageBreaks="1" fitToPage="1" printArea="1">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup scale="80" fitToHeight="0" orientation="landscape" r:id="rId2"/>
+      <headerFooter>
+        <oddHeader>&amp;C&amp;"Calibri,Regular"&amp;K000000CSC - DRAFT - VER6c_x000D_FOR PUBLIC COMMENT ONLY</oddHeader>
+        <oddFooter>&amp;C&amp;"Calibri,Regular"&amp;K000000CSC - DRAFT - VER6c_x000D_FOR PUBLIC COMMENT ONLY</oddFooter>
+      </headerFooter>
+    </customSheetView>
+    <customSheetView guid="{FB597F9D-3EB9-9C48-BC71-4C09FB1B9DF4}" scale="90" showPageBreaks="1" fitToPage="1" printArea="1">
+      <pane ySplit="3.0625" topLeftCell="A4" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup scale="82" fitToHeight="0" orientation="landscape"/>
+      <headerFooter>
+        <oddHeader>&amp;C&amp;"Calibri,Regular"&amp;K000000CSC - DRAFT - VER6c_x000D_FOR PUBLIC COMMENT ONLY</oddHeader>
+        <oddFooter>&amp;C&amp;"Calibri,Regular"&amp;K000000CSC - DRAFT - VER6c_x000D_FOR PUBLIC COMMENT ONLY</oddFooter>
+      </headerFooter>
+    </customSheetView>
+    <customSheetView guid="{784EFDF6-DF57-4744-A1FE-569B86C0D3A6}" scale="90" fitToPage="1" printArea="1">
+      <pane ySplit="2" topLeftCell="A88" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="D97" sqref="D97"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <pageSetup scale="76" fitToHeight="0" orientation="landscape"/>
       <headerFooter>
         <oddHeader>&amp;C&amp;"Calibri,Regular"&amp;K000000CSC - DRAFT - VER6c_x000D_FOR PUBLIC COMMENT ONLY</oddHeader>
         <oddFooter>&amp;C&amp;"Calibri,Regular"&amp;K000000CSC - DRAFT - VER6c_x000D_FOR PUBLIC COMMENT ONLY</oddFooter>
@@ -10023,29 +10679,9 @@
         <oddFooter>&amp;C&amp;"Calibri,Regular"&amp;K000000CSC - DRAFT - VER6c_x000D_FOR PUBLIC COMMENT ONLY</oddFooter>
       </headerFooter>
     </customSheetView>
-    <customSheetView guid="{784EFDF6-DF57-4744-A1FE-569B86C0D3A6}" scale="90" fitToPage="1" printArea="1">
-      <pane ySplit="2" topLeftCell="A88" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D97" sqref="D97"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup scale="76" fitToHeight="0" orientation="landscape"/>
-      <headerFooter>
-        <oddHeader>&amp;C&amp;"Calibri,Regular"&amp;K000000CSC - DRAFT - VER6c_x000D_FOR PUBLIC COMMENT ONLY</oddHeader>
-        <oddFooter>&amp;C&amp;"Calibri,Regular"&amp;K000000CSC - DRAFT - VER6c_x000D_FOR PUBLIC COMMENT ONLY</oddFooter>
-      </headerFooter>
-    </customSheetView>
-    <customSheetView guid="{FB597F9D-3EB9-9C48-BC71-4C09FB1B9DF4}" scale="90" showPageBreaks="1" fitToPage="1" printArea="1">
-      <pane ySplit="3.0625" topLeftCell="A4" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup scale="82" fitToHeight="0" orientation="landscape"/>
-      <headerFooter>
-        <oddHeader>&amp;C&amp;"Calibri,Regular"&amp;K000000CSC - DRAFT - VER6c_x000D_FOR PUBLIC COMMENT ONLY</oddHeader>
-        <oddFooter>&amp;C&amp;"Calibri,Regular"&amp;K000000CSC - DRAFT - VER6c_x000D_FOR PUBLIC COMMENT ONLY</oddFooter>
-      </headerFooter>
-    </customSheetView>
-    <customSheetView guid="{156F6E94-B77C-4218-9566-01A2D0E67E8E}" scale="90" showPageBreaks="1" fitToPage="1" printArea="1">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+    <customSheetView guid="{166C989B-D112-4FBE-9337-483856443AEC}" scale="85" fitToPage="1" printArea="1" topLeftCell="B1">
+      <pane ySplit="3" topLeftCell="A144" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="H147" sqref="H147"/>
       <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup scale="80" fitToHeight="0" orientation="landscape" r:id="rId3"/>
       <headerFooter>
@@ -10053,8 +10689,29 @@
         <oddFooter>&amp;C&amp;"Calibri,Regular"&amp;K000000CSC - DRAFT - VER6c_x000D_FOR PUBLIC COMMENT ONLY</oddFooter>
       </headerFooter>
     </customSheetView>
+    <customSheetView guid="{9FD8CC1C-6420-44A1-A370-C19CD963FBCC}" scale="85" showPageBreaks="1" fitToPage="1" printArea="1" showAutoFilter="1">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup fitToHeight="0" orientation="landscape" r:id="rId4"/>
+      <headerFooter>
+        <oddHeader>&amp;C&amp;"Calibri,Regular"&amp;K000000CSC - DRAFT - VER6c_x000D_FOR PUBLIC COMMENT ONLY</oddHeader>
+        <oddFooter>&amp;C&amp;"Calibri,Regular"&amp;K000000CSC - DRAFT - VER6c_x000D_FOR PUBLIC COMMENT ONLY</oddFooter>
+      </headerFooter>
+      <autoFilter ref="A3:H172"/>
+    </customSheetView>
   </customSheetViews>
   <mergeCells count="20">
+    <mergeCell ref="C97:E97"/>
+    <mergeCell ref="C86:E86"/>
+    <mergeCell ref="C78:E78"/>
+    <mergeCell ref="C164:E164"/>
+    <mergeCell ref="C156:E156"/>
+    <mergeCell ref="C146:E146"/>
+    <mergeCell ref="C140:E140"/>
+    <mergeCell ref="C125:E125"/>
+    <mergeCell ref="C107:E107"/>
+    <mergeCell ref="C115:E115"/>
     <mergeCell ref="C4:E4"/>
     <mergeCell ref="C73:E73"/>
     <mergeCell ref="C66:E66"/>
@@ -10065,28 +10722,13 @@
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="C11:E11"/>
     <mergeCell ref="C50:E50"/>
-    <mergeCell ref="C97:E97"/>
-    <mergeCell ref="C86:E86"/>
-    <mergeCell ref="C78:E78"/>
-    <mergeCell ref="C164:E164"/>
-    <mergeCell ref="C156:E156"/>
-    <mergeCell ref="C146:E146"/>
-    <mergeCell ref="C140:E140"/>
-    <mergeCell ref="C125:E125"/>
-    <mergeCell ref="C107:E107"/>
-    <mergeCell ref="C115:E115"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup fitToHeight="0" orientation="landscape" r:id="rId4"/>
+  <pageSetup fitToHeight="0" orientation="landscape" r:id="rId5"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Calibri,Regular"&amp;K000000CSC - DRAFT - VER6c_x000D_FOR PUBLIC COMMENT ONLY</oddHeader>
     <oddFooter>&amp;C&amp;"Calibri,Regular"&amp;K000000CSC - DRAFT - VER6c_x000D_FOR PUBLIC COMMENT ONLY</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added the cis and nist version to the cis tag and nist tag
Signed-off-by: dromazmj <dromazmj@dukes.jmu.edu>
</commit_message>
<xml_diff>
--- a/data/NIST_Map_09212017B_CSC-CIS_Critical_Security_Controls_VER_6.1_Excel_9.1.2016.xlsx
+++ b/data/NIST_Map_09212017B_CSC-CIS_Critical_Security_Controls_VER_6.1_Excel_9.1.2016.xlsx
@@ -2184,168 +2184,6 @@
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
 <headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{2F8F7620-4C4F-A040-A1DD-B07BF2744515}" diskRevisions="1" revisionId="863" version="10">
-  <header guid="{5EC76917-8FE5-4B58-BD6B-154862C439F5}" dateTime="2017-09-20T09:12:56" maxSheetId="3" userName="Haynes, Dan" r:id="rId33">
-    <sheetIdMap count="2">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{EC0A1B06-3529-4AA8-B581-4EED1D8ACBAE}" dateTime="2017-09-20T15:00:16" maxSheetId="3" userName="Haynes, Dan" r:id="rId34" minRId="559" maxRId="560">
-    <sheetIdMap count="2">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{AC011676-9FB9-43B0-81EF-2DD2C38DB95E}" dateTime="2017-09-20T15:00:48" maxSheetId="3" userName="Haynes, Dan" r:id="rId35" minRId="562">
-    <sheetIdMap count="2">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{BCA57637-F52B-4E32-B407-B5CC193FB99A}" dateTime="2017-09-20T15:01:21" maxSheetId="3" userName="Haynes, Dan" r:id="rId36" minRId="563">
-    <sheetIdMap count="2">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{D79C9C3D-BF37-438D-B5BD-4967FA4A87F4}" dateTime="2017-09-20T15:02:03" maxSheetId="3" userName="Haynes, Dan" r:id="rId37" minRId="564">
-    <sheetIdMap count="2">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{53B7C958-3630-4716-816D-46B70A1DB4F9}" dateTime="2017-09-20T15:42:19" maxSheetId="3" userName="Haynes, Dan" r:id="rId38" minRId="565">
-    <sheetIdMap count="2">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{04B436EA-8B77-41BD-A2D8-691A12C9B565}" dateTime="2017-09-20T15:43:45" maxSheetId="3" userName="Haynes, Dan" r:id="rId39" minRId="567">
-    <sheetIdMap count="2">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{0E37CAD3-F66B-4E46-91A4-20A86E2DBE85}" dateTime="2017-09-20T18:49:47" maxSheetId="3" userName="Haynes, Dan" r:id="rId40" minRId="568">
-    <sheetIdMap count="2">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{A8AAC16C-21BF-4614-A5CA-B3DF028F49F3}" dateTime="2017-09-20T18:57:10" maxSheetId="3" userName="Haynes, Dan" r:id="rId41" minRId="569">
-    <sheetIdMap count="2">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{5D8DF038-4CF9-46A4-A9EB-EB05E7D88C18}" dateTime="2017-09-20T18:58:49" maxSheetId="3" userName="Haynes, Dan" r:id="rId42" minRId="570" maxRId="571">
-    <sheetIdMap count="2">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{38F8DC5C-7562-4656-BADF-8E2F3AB1AF26}" dateTime="2017-09-20T19:02:36" maxSheetId="3" userName="Haynes, Dan" r:id="rId43" minRId="572" maxRId="573">
-    <sheetIdMap count="2">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{E7158350-5139-45D4-B29C-11F30D4EDA67}" dateTime="2017-09-20T19:25:12" maxSheetId="3" userName="Haynes, Dan" r:id="rId44" minRId="574">
-    <sheetIdMap count="2">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{625EEFC7-7E42-4D25-A02A-3645BC12A959}" dateTime="2017-09-20T19:37:09" maxSheetId="3" userName="Haynes, Dan" r:id="rId45" minRId="576" maxRId="578">
-    <sheetIdMap count="2">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{85272046-6A4A-4044-B8A3-3FC9A64BD173}" dateTime="2017-09-20T19:47:35" maxSheetId="3" userName="Haynes, Dan" r:id="rId46" minRId="580" maxRId="581">
-    <sheetIdMap count="2">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{68674675-3D1C-4999-A137-413ECB81E6AE}" dateTime="2017-09-20T19:50:21" maxSheetId="3" userName="Haynes, Dan" r:id="rId47" minRId="582" maxRId="583">
-    <sheetIdMap count="2">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{ACF6F627-648D-4A71-A20C-1C906EA9BF92}" dateTime="2017-09-21T00:52:35" maxSheetId="3" userName="Aronne, Eugene J." r:id="rId48" minRId="584" maxRId="607">
-    <sheetIdMap count="2">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{27D4038E-29A1-4DD6-9282-81165E1E3FE0}" dateTime="2017-09-21T01:41:12" maxSheetId="3" userName="Aronne, Eugene J." r:id="rId49" minRId="608" maxRId="638">
-    <sheetIdMap count="2">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{FC8E0454-76E7-49A0-AC04-FEA9396126B0}" dateTime="2017-09-21T01:42:14" maxSheetId="3" userName="Aronne, Eugene J." r:id="rId50">
-    <sheetIdMap count="2">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{EBDE4F6B-CA0D-4B4D-88BA-82D84424E96F}" dateTime="2017-09-21T01:55:14" maxSheetId="3" userName="Aronne, Eugene J." r:id="rId51" minRId="640" maxRId="653">
-    <sheetIdMap count="2">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{11758A7C-593E-4704-A9E7-9961199DEDE9}" dateTime="2017-09-21T02:29:39" maxSheetId="3" userName="Aronne, Eugene J." r:id="rId52" minRId="654" maxRId="701">
-    <sheetIdMap count="2">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{E94E4A38-4A9B-4645-B343-8F4ABDDAE345}" dateTime="2017-09-21T08:26:51" maxSheetId="3" userName="Aronne, Eugene J." r:id="rId53" minRId="702" maxRId="750">
-    <sheetIdMap count="2">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{FBCC78D9-CE81-4594-B214-32C053863122}" dateTime="2017-09-21T11:39:30" maxSheetId="3" userName="Aronne, Eugene J." r:id="rId54" minRId="753" maxRId="772">
-    <sheetIdMap count="2">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{BD941FF8-A8CC-4E54-9AC8-21089DEA56FF}" dateTime="2017-09-21T11:57:59" maxSheetId="3" userName="Aronne, Eugene J." r:id="rId55" minRId="773" maxRId="786">
-    <sheetIdMap count="2">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{87D1514F-CC39-48DD-AE15-1B806720FE63}" dateTime="2017-09-21T11:59:26" maxSheetId="3" userName="Aronne, Eugene J." r:id="rId56" minRId="787" maxRId="788">
-    <sheetIdMap count="2">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{DE541A0D-B10F-43E9-A869-4A9BEBA82711}" dateTime="2017-09-21T12:00:40" maxSheetId="3" userName="Aronne, Eugene J." r:id="rId57" minRId="791" maxRId="792">
-    <sheetIdMap count="2">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{E83CBE03-383D-4948-868C-0921010DAE44}" dateTime="2017-09-21T12:02:15" maxSheetId="3" userName="Aronne, Eugene J." r:id="rId58" minRId="795" maxRId="796">
-    <sheetIdMap count="2">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-    </sheetIdMap>
-  </header>
-  <header guid="{8F2E6932-4BDA-47C6-B56B-B50AF3BFD155}" dateTime="2017-09-21T12:05:53" maxSheetId="3" userName="Aronne, Eugene J." r:id="rId59" minRId="799" maxRId="808">
-    <sheetIdMap count="2">
-      <sheetId val="1"/>
-      <sheetId val="2"/>
-    </sheetIdMap>
-  </header>
   <header guid="{6663B3B2-0172-4D31-B8DB-D15A051B9192}" dateTime="2017-09-21T12:09:56" maxSheetId="3" userName="Aronne, Eugene J." r:id="rId60">
     <sheetIdMap count="2">
       <sheetId val="1"/>
@@ -2359,3628 +2197,6 @@
     </sheetIdMap>
   </header>
 </headers>
-</file>
-
-<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rfmt sheetId="2" sqref="A67:XFD67">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="2" sqref="A108:XFD108">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="2" sqref="A109:XFD109">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="2" sqref="A111:XFD113">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="2" sqref="A129:XFD129">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="2" sqref="A147:XFD147">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </rfmt>
-  <rcc rId="559" sId="2">
-    <nc r="A147" t="inlineStr">
-      <is>
-        <t xml:space="preserve">CM-2, </t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="560" sId="2">
-    <nc r="A67" t="inlineStr">
-      <is>
-        <t>CM-7</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcv guid="{166C989B-D112-4FBE-9337-483856443AEC}" action="delete"/>
-  <rdn rId="0" localSheetId="2" customView="1" name="Z_166C989B_D112_4FBE_9337_483856443AEC_.wvu.PrintArea" hidden="1" oldHidden="1">
-    <formula>'VER 6.1 Controls'!$C$3:$E$172</formula>
-    <oldFormula>'VER 6.1 Controls'!$C$3:$E$172</oldFormula>
-  </rdn>
-  <rcv guid="{166C989B-D112-4FBE-9337-483856443AEC}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog10.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rfmt sheetId="2" sqref="H1:H1048576">
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="2" sqref="H1:H1048576">
-    <dxf>
-      <alignment vertical="top"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="2" sqref="H1:H1048576">
-    <dxf>
-      <alignment horizontal="left"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="572" sId="2">
-    <nc r="A109" t="inlineStr">
-      <is>
-        <t>SC-8</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="573" sId="2">
-    <nc r="A112" t="inlineStr">
-      <is>
-        <t>SC-28</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog11.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="574" sId="2">
-    <nc r="A113" t="inlineStr">
-      <is>
-        <t>AU-2</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcv guid="{166C989B-D112-4FBE-9337-483856443AEC}" action="delete"/>
-  <rdn rId="0" localSheetId="2" customView="1" name="Z_166C989B_D112_4FBE_9337_483856443AEC_.wvu.PrintArea" hidden="1" oldHidden="1">
-    <formula>'VER 6.1 Controls'!$C$3:$E$172</formula>
-    <oldFormula>'VER 6.1 Controls'!$C$3:$E$172</oldFormula>
-  </rdn>
-  <rcv guid="{166C989B-D112-4FBE-9337-483856443AEC}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog12.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="576" sId="2">
-    <oc r="H67" t="inlineStr">
-      <is>
-        <t>(4) UNAUTHORIZED SOFWTARE /BLACKLISTING</t>
-      </is>
-    </oc>
-    <nc r="H67"/>
-  </rcc>
-  <rcc rId="577" sId="2">
-    <oc r="A147" t="inlineStr">
-      <is>
-        <t xml:space="preserve">CM-2, </t>
-      </is>
-    </oc>
-    <nc r="A147" t="inlineStr">
-      <is>
-        <t>SI-2</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="578" sId="2">
-    <nc r="H147" t="inlineStr">
-      <is>
-        <t>CM-2 may also be related, but, SI-2 actually talks about keeping software patched and up-to-date to address flaws.</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcv guid="{166C989B-D112-4FBE-9337-483856443AEC}" action="delete"/>
-  <rdn rId="0" localSheetId="2" customView="1" name="Z_166C989B_D112_4FBE_9337_483856443AEC_.wvu.PrintArea" hidden="1" oldHidden="1">
-    <formula>'VER 6.1 Controls'!$C$3:$E$172</formula>
-    <oldFormula>'VER 6.1 Controls'!$C$3:$E$172</oldFormula>
-  </rdn>
-  <rcv guid="{166C989B-D112-4FBE-9337-483856443AEC}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog13.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="580" sId="2">
-    <nc r="A129" t="inlineStr">
-      <is>
-        <t>AC-2 (5)</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="581" sId="2">
-    <nc r="H111" t="inlineStr">
-      <is>
-        <t>ac-3, mp-4, sc-28</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog14.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="582" sId="2">
-    <oc r="H111" t="inlineStr">
-      <is>
-        <t>ac-3, mp-4, sc-28</t>
-      </is>
-    </oc>
-    <nc r="H111"/>
-  </rcc>
-  <rcc rId="583" sId="2">
-    <nc r="A111" t="inlineStr">
-      <is>
-        <t>AC-3 (3)</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog15.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="584" sId="2">
-    <oc r="B67" t="inlineStr">
-      <is>
-        <t>LEAST FUNCTIONALITY</t>
-      </is>
-    </oc>
-    <nc r="B67" t="inlineStr">
-      <is>
-        <r>
-          <t xml:space="preserve">LEAST FUNCTIONALITY </t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color rgb="FFFF0000"/>
-            <rFont val="Calibri"/>
-            <family val="2"/>
-          </rPr>
-          <t>| PERIODIC REVIEW</t>
-        </r>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="585" sId="2">
-    <nc r="B108" t="inlineStr">
-      <is>
-        <t>INFORMATION FLOW ENFORCEMENT</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="586" sId="2" xfDxf="1" dxf="1">
-    <nc r="B109" t="inlineStr">
-      <is>
-        <t>TRANSMISSION CONFIDENTIALITY AND INTEGRITY</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </ndxf>
-  </rcc>
-  <rfmt sheetId="2" sqref="B109 B108" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="587" sId="2" xfDxf="1" dxf="1">
-    <nc r="B111" t="inlineStr">
-      <is>
-        <t>ACCESS ENFORCEMENT | MANDATORY ACCESS CONTROL</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </ndxf>
-  </rcc>
-  <rfmt sheetId="2" sqref="B111" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="588" sId="2" xfDxf="1" dxf="1">
-    <nc r="B112" t="inlineStr">
-      <is>
-        <t>PROTECTION OF INFORMATION AT REST</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </ndxf>
-  </rcc>
-  <rfmt sheetId="2" sqref="B112" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="589" sId="2" odxf="1" dxf="1">
-    <nc r="B113" t="inlineStr">
-      <is>
-        <t>AUDIT EVENTS</t>
-      </is>
-    </nc>
-    <odxf>
-      <font>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-    </odxf>
-    <ndxf>
-      <font>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </ndxf>
-  </rcc>
-  <rcc rId="590" sId="2" xfDxf="1" dxf="1">
-    <nc r="B129" t="inlineStr">
-      <is>
-        <t>ACCOUNT MANAGEMENT | INACTIVITY LOGOUT</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </ndxf>
-  </rcc>
-  <rfmt sheetId="2" sqref="B129" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="591" sId="2">
-    <nc r="B147" t="inlineStr">
-      <is>
-        <t>FLAW REMEDIATION</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="B147" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="592" sId="2">
-    <nc r="A51" t="inlineStr">
-      <is>
-        <t>SI-2</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="593" sId="2">
-    <nc r="B51" t="inlineStr">
-      <is>
-        <t>FLAW REMEDIATION</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="594" sId="2">
-    <nc r="A52" t="inlineStr">
-      <is>
-        <t>CM-7</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="595" sId="2">
-    <nc r="B52" t="inlineStr">
-      <is>
-        <t>LEAST FUNCTIONALITY</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="596" sId="2">
-    <nc r="A53" t="inlineStr">
-      <is>
-        <t>CM-7</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="597" sId="2">
-    <nc r="B53" t="inlineStr">
-      <is>
-        <t>LEAST FUNCTIONALITY</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="598" sId="2">
-    <nc r="A54" t="inlineStr">
-      <is>
-        <t>SI-4</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="599" sId="2">
-    <nc r="B54" t="inlineStr">
-      <is>
-        <t>INFORMATION SYSTEM MONITORING</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="600" sId="2">
-    <nc r="A55" t="inlineStr">
-      <is>
-        <t>CM-7</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="601" sId="2">
-    <nc r="B55" t="inlineStr">
-      <is>
-        <t>LEAST FUNCTIONALITY</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="602" sId="2">
-    <nc r="A56" t="inlineStr">
-      <is>
-        <t>SC-7</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="603" sId="2">
-    <nc r="B56" t="inlineStr">
-      <is>
-        <t>BOUNDARY PROTECTION</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="604" sId="2">
-    <nc r="A57" t="inlineStr">
-      <is>
-        <t>SI-3</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="605" sId="2">
-    <nc r="B57" t="inlineStr">
-      <is>
-        <t>MALICIOUS CODE PROTECTION</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="606" sId="2">
-    <nc r="A58" t="inlineStr">
-      <is>
-        <t>SI-3</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="607" sId="2">
-    <nc r="B58" t="inlineStr">
-      <is>
-        <t>MALICIOUS CODE PROTECTION</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="A51:B58" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog16.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rfmt sheetId="2" xfDxf="1" sqref="B60" start="0" length="0">
-    <dxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </dxf>
-  </rfmt>
-  <rcc rId="608" sId="2" xfDxf="1" dxf="1">
-    <nc r="B61" t="inlineStr">
-      <is>
-        <t>MALICIOUS CODE PROTECTION | AUTOMATIC UPDATES</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </ndxf>
-  </rcc>
-  <rcc rId="609" sId="2">
-    <nc r="A61" t="inlineStr">
-      <is>
-        <t>SI-3(2)</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="610" sId="2">
-    <nc r="A60" t="inlineStr">
-      <is>
-        <t>SI-3</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="611" sId="2">
-    <nc r="B60" t="inlineStr">
-      <is>
-        <t>MALICIOUS CODE PROTECTION</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="612" sId="2">
-    <nc r="A62" t="inlineStr">
-      <is>
-        <t>SI-4</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="613" sId="2" xfDxf="1" dxf="1">
-    <nc r="B62" t="inlineStr">
-      <is>
-        <t>INFORMATION SYSTEM MONITORING</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </ndxf>
-  </rcc>
-  <rfmt sheetId="2" sqref="A60:B62" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="614" sId="2">
-    <nc r="A63" t="inlineStr">
-      <is>
-        <t>SI-16</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="615" sId="2" xfDxf="1" dxf="1">
-    <nc r="B63" t="inlineStr">
-      <is>
-        <t>MEMORY PROTECTION</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </ndxf>
-  </rcc>
-  <rfmt sheetId="2" sqref="A63:B63" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="616" sId="2">
-    <nc r="A64" t="inlineStr">
-      <is>
-        <t>SI-3</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="617" sId="2" odxf="1" dxf="1">
-    <nc r="B64" t="inlineStr">
-      <is>
-        <t>MALICIOUS CODE PROTECTION</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </ndxf>
-  </rcc>
-  <rcc rId="618" sId="2">
-    <nc r="A65" t="inlineStr">
-      <is>
-        <t>AU-2</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="619" sId="2">
-    <nc r="B65" t="inlineStr">
-      <is>
-        <t>AUDIT EVENTS</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="A65:B65" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="2" sqref="A64" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="620" sId="2" xfDxf="1" dxf="1">
-    <nc r="B68" t="inlineStr">
-      <is>
-        <t>BOUNDARY PROTECTION | DENY BY DEFAULT / ALLOW BY EXCEPTION</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </ndxf>
-  </rcc>
-  <rcc rId="621" sId="2">
-    <nc r="A68" t="inlineStr">
-      <is>
-        <t>SC-7(5)</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="622" sId="2">
-    <oc r="A67" t="inlineStr">
-      <is>
-        <t>CM-7 (1)</t>
-      </is>
-    </oc>
-    <nc r="A67" t="inlineStr">
-      <is>
-        <t>CM-7(1)</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="A68:B68" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="623" sId="2">
-    <nc r="A69" t="inlineStr">
-      <is>
-        <t>RA-5</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="624" sId="2" xfDxf="1" dxf="1">
-    <nc r="B69" t="inlineStr">
-      <is>
-        <t>VULNERABILITY SCANNING</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </ndxf>
-  </rcc>
-  <rfmt sheetId="2" sqref="A69:B69" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="625" sId="2">
-    <nc r="A72" t="inlineStr">
-      <is>
-        <t>SI-10</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="626" sId="2" xfDxf="1" dxf="1">
-    <nc r="B72" t="inlineStr">
-      <is>
-        <t>INFORMATION INPUT VALIDATION</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </ndxf>
-  </rcc>
-  <rcc rId="627" sId="2">
-    <nc r="A71" t="inlineStr">
-      <is>
-        <t>CM-7</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="628" sId="2">
-    <nc r="B71" t="inlineStr">
-      <is>
-        <t>LEAST FUNCTIONALITY</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="629" sId="2">
-    <nc r="A70" t="inlineStr">
-      <is>
-        <t>SC-7</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="630" sId="2">
-    <nc r="B70" t="inlineStr">
-      <is>
-        <t>BOUNDARY PROTECTION</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="A70:B72" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="631" sId="2">
-    <nc r="A74" t="inlineStr">
-      <is>
-        <t>CP-9</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="632" sId="2">
-    <nc r="B74" t="inlineStr">
-      <is>
-        <t>INFORMATION SYSTEM BACKUP</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="633" sId="2" xfDxf="1" dxf="1">
-    <nc r="B75" t="inlineStr">
-      <is>
-        <t>INFORMATION SYSTEM BACKUP | TESTING FOR RELIABILITY / INTEGRITY</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </ndxf>
-  </rcc>
-  <rcc rId="634" sId="2">
-    <nc r="A75" t="inlineStr">
-      <is>
-        <t>CP-9(1)</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="635" sId="2" xfDxf="1" dxf="1">
-    <nc r="B77" t="inlineStr">
-      <is>
-        <t>INFORMATION SYSTEM BACKUP | SEPARATE STORAGE FOR CRITICAL INFORMATION</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </ndxf>
-  </rcc>
-  <rcc rId="636" sId="2">
-    <nc r="A77" t="inlineStr">
-      <is>
-        <t>CP-9(3)</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="637" sId="2">
-    <nc r="A76" t="inlineStr">
-      <is>
-        <t>CP-9</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="638" sId="2">
-    <nc r="B76" t="inlineStr">
-      <is>
-        <t>INFORMATION SYSTEM BACKUP</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="A74:B77" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog17.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rfmt sheetId="2" sqref="A1:A172" start="0" length="0">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="2" sqref="A1:G1" start="0" length="0">
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="2" sqref="G1:G172" start="0" length="0">
-    <dxf>
-      <border>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="2" sqref="A172:G172" start="0" length="0">
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="2" sqref="A1:G172">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-  </rfmt>
-  <rcv guid="{9FD8CC1C-6420-44A1-A370-C19CD963FBCC}" action="delete"/>
-  <rdn rId="0" localSheetId="2" customView="1" name="Z_9FD8CC1C_6420_44A1_A370_C19CD963FBCC_.wvu.PrintArea" hidden="1" oldHidden="1">
-    <formula>'VER 6.1 Controls'!$C$3:$E$172</formula>
-    <oldFormula>'VER 6.1 Controls'!$C$3:$E$172</oldFormula>
-  </rdn>
-  <rcv guid="{9FD8CC1C-6420-44A1-A370-C19CD963FBCC}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog18.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rfmt sheetId="2" sqref="E1:E1048576">
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="2" sqref="E1:E1048576">
-    <dxf>
-      <alignment vertical="top"/>
-    </dxf>
-  </rfmt>
-  <rdn rId="0" localSheetId="2" customView="1" name="Z_166C989B_D112_4FBE_9337_483856443AEC_.wvu.PrintArea" hidden="1" oldHidden="1">
-    <formula>'VER 6.1 Controls'!$C$3:$E$172</formula>
-  </rdn>
-  <rcv guid="{166C989B-D112-4FBE-9337-483856443AEC}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog19.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="640" sId="2">
-    <nc r="B83" t="inlineStr">
-      <is>
-        <t>FLAW REMEDIATION</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="641" sId="2">
-    <nc r="A83" t="inlineStr">
-      <is>
-        <t>SI-2</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="642" sId="2">
-    <nc r="A82" t="inlineStr">
-      <is>
-        <t>SC-23</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="643" sId="2">
-    <nc r="B82" t="inlineStr">
-      <is>
-        <t>SESSION AUTHENTICITY</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="644" sId="2" xfDxf="1" dxf="1">
-    <nc r="B81" t="inlineStr">
-      <is>
-        <t>CONFIGURATION SETTINGS | RESPOND TO UNAUTHORIZED CHANGES</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </ndxf>
-  </rcc>
-  <rcc rId="645" sId="2">
-    <nc r="A81" t="inlineStr">
-      <is>
-        <t>CM-6(2)</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="646" sId="2" xfDxf="1" dxf="1">
-    <nc r="B79" t="inlineStr">
-      <is>
-        <t>CONFIGURATION SETTINGS | AUTOMATED CENTRAL MANAGEMENT / APPLICATION / VERIFICATION</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </ndxf>
-  </rcc>
-  <rcc rId="647" sId="2">
-    <nc r="A79" t="inlineStr">
-      <is>
-        <t>CM-6(1)</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="648" sId="2" xfDxf="1" dxf="1">
-    <nc r="B80" t="inlineStr">
-      <is>
-        <t>INFORMATION SYSTEM COMPONENT INVENTORY | ASSESSED CONFIGURATIONS / APPROVED DEVIATIONS</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </ndxf>
-  </rcc>
-  <rcc rId="649" sId="2">
-    <nc r="A80" t="inlineStr">
-      <is>
-        <t>CM-8(6)</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="A79:B85" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="2" xfDxf="1" sqref="B84" start="0" length="0">
-    <dxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-  </rfmt>
-  <rcc rId="650" sId="2">
-    <nc r="B84" t="inlineStr">
-      <is>
-        <t>APPLICATION PARTITIONING</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="651" sId="2">
-    <nc r="A84" t="inlineStr">
-      <is>
-        <t>SC-2</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="652" sId="2">
-    <nc r="A85" t="inlineStr">
-      <is>
-        <t>SC-2</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="653" sId="2">
-    <nc r="B85" t="inlineStr">
-      <is>
-        <t>APPLICATION PARTITIONING</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="562" sId="2">
-    <nc r="B67" t="inlineStr">
-      <is>
-        <t>LEAST FUNCTIONALITY</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog20.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="654" sId="2">
-    <nc r="A170" t="inlineStr">
-      <is>
-        <t>RA-5</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="655" sId="2">
-    <nc r="A165" t="inlineStr">
-      <is>
-        <t>CA-8</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="656" sId="2">
-    <nc r="B165" t="inlineStr">
-      <is>
-        <t>PENETRATION TESTING</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="657" sId="2">
-    <nc r="A166" t="inlineStr">
-      <is>
-        <t>CA-8</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="658" sId="2">
-    <nc r="B166" t="inlineStr">
-      <is>
-        <t>PENETRATION TESTING</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="659" sId="2">
-    <nc r="A168" t="inlineStr">
-      <is>
-        <t>CA-8</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="660" sId="2">
-    <nc r="B168" t="inlineStr">
-      <is>
-        <t>PENETRATION TESTING</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="661" sId="2">
-    <nc r="A169" t="inlineStr">
-      <is>
-        <t>CA-8</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="662" sId="2">
-    <nc r="B169" t="inlineStr">
-      <is>
-        <t>PENETRATION TESTING</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="663" sId="2">
-    <nc r="B170" t="inlineStr">
-      <is>
-        <t>VULNERABILITY SCANNING</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="664" sId="2" xfDxf="1" dxf="1">
-    <nc r="B171" t="inlineStr">
-      <is>
-        <t>PENETRATION TESTING | RED TEAM EXERCISES</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </ndxf>
-  </rcc>
-  <rcc rId="665" sId="2">
-    <nc r="A171" t="inlineStr">
-      <is>
-        <t>CA-8(2)</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="666" sId="2" xfDxf="1" dxf="1">
-    <nc r="B167" t="inlineStr">
-      <is>
-        <t>PENETRATION TESTING | RED TEAM EXERCISES</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </ndxf>
-  </rcc>
-  <rcc rId="667" sId="2">
-    <nc r="A167" t="inlineStr">
-      <is>
-        <t>CA-8(2)</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="668" sId="2">
-    <nc r="A172" t="inlineStr">
-      <is>
-        <t>CA-8</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="669" sId="2">
-    <nc r="B172" t="inlineStr">
-      <is>
-        <t>PENETRATION TESTING</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="A165:B172" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="670" sId="2">
-    <nc r="A157" t="inlineStr">
-      <is>
-        <t>IR-1</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="671" sId="2">
-    <nc r="B157" t="inlineStr">
-      <is>
-        <t>INCIDENT RESPONSE POLICY AND PROCEDURES</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="672" sId="2" xfDxf="1" dxf="1">
-    <nc r="B163" t="inlineStr">
-      <is>
-        <t>INCIDENT RESPONSE TRAINING</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </ndxf>
-  </rcc>
-  <rcc rId="673" sId="2">
-    <nc r="A163" t="inlineStr">
-      <is>
-        <t>IR-2</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="674" sId="2">
-    <nc r="A159" t="inlineStr">
-      <is>
-        <t>IR-4</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="675" sId="2">
-    <nc r="B159" t="inlineStr">
-      <is>
-        <t>INCIDENT HANDLING</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="676" sId="2">
-    <nc r="A158" t="inlineStr">
-      <is>
-        <t>IR-4</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="677" sId="2">
-    <nc r="B158" t="inlineStr">
-      <is>
-        <t>INCIDENT HANDLING</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="678" sId="2">
-    <nc r="A160" t="inlineStr">
-      <is>
-        <t>IR-6</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="679" sId="2">
-    <nc r="B160" t="inlineStr">
-      <is>
-        <t>INCIDENT REPORTING</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="680" sId="2">
-    <nc r="A161" t="inlineStr">
-      <is>
-        <t>IR-6</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="681" sId="2">
-    <nc r="B161" t="inlineStr">
-      <is>
-        <t>INCIDENT REPORTING</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="682" sId="2">
-    <nc r="A162" t="inlineStr">
-      <is>
-        <t>IR-2</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="683" sId="2">
-    <nc r="B162" t="inlineStr">
-      <is>
-        <t>INCIDENT RESPONSE TRAINING</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="A157:B163" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="684" sId="2" xfDxf="1" dxf="1">
-    <nc r="B117" t="inlineStr">
-      <is>
-        <t>INFORMATION SYSTEM MONITORING | WIRELESS INTRUSION DETECTION</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </ndxf>
-  </rcc>
-  <rcc rId="685" sId="2">
-    <nc r="B118" t="inlineStr">
-      <is>
-        <t>INFORMATION SYSTEM MONITORING | WIRELESS INTRUSION DETECTION</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="686" sId="2">
-    <nc r="A117" t="inlineStr">
-      <is>
-        <t>SI-4(14)</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="687" sId="2">
-    <nc r="A118" t="inlineStr">
-      <is>
-        <t>SI-4(14)</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="A117:B118" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="688" sId="2" xfDxf="1" dxf="1">
-    <nc r="B128" t="inlineStr">
-      <is>
-        <t>PERSONNEL TERMINATION</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </ndxf>
-  </rcc>
-  <rcc rId="689" sId="2">
-    <nc r="A128" t="inlineStr">
-      <is>
-        <t>PS-4</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="690" sId="2" xfDxf="1" dxf="1">
-    <nc r="B126" t="inlineStr">
-      <is>
-        <t>IDENTIFIER MANAGEMENT</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </ndxf>
-  </rcc>
-  <rcc rId="691" sId="2" xfDxf="1" dxf="1">
-    <nc r="B127" t="inlineStr">
-      <is>
-        <t>IDENTIFIER MANAGEMENT</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </ndxf>
-  </rcc>
-  <rcc rId="692" sId="2">
-    <nc r="A126" t="inlineStr">
-      <is>
-        <t>IA-4</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="693" sId="2">
-    <nc r="A127" t="inlineStr">
-      <is>
-        <t>IA-4</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="694" sId="2">
-    <nc r="A130" t="inlineStr">
-      <is>
-        <t>AC-11</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="695" sId="2">
-    <nc r="B130" t="inlineStr">
-      <is>
-        <t>SESSION LOCK</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="A126:B128 A130:B130" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="696" sId="2" odxf="1" dxf="1">
-    <nc r="A131" t="inlineStr">
-      <is>
-        <t>IA-4</t>
-      </is>
-    </nc>
-    <odxf>
-      <font>
-        <family val="2"/>
-      </font>
-    </odxf>
-    <ndxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </ndxf>
-  </rcc>
-  <rcc rId="697" sId="2" odxf="1" dxf="1">
-    <nc r="B131" t="inlineStr">
-      <is>
-        <t>IDENTIFIER MANAGEMENT</t>
-      </is>
-    </nc>
-    <odxf>
-      <font>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-    </odxf>
-    <ndxf>
-      <font>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </ndxf>
-  </rcc>
-  <rcc rId="698" sId="2">
-    <nc r="A132" t="inlineStr">
-      <is>
-        <t>AC-7</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="699" sId="2" xfDxf="1" dxf="1">
-    <nc r="B132" t="inlineStr">
-      <is>
-        <t>UNSUCCESSFUL LOGON ATTEMPTS</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </ndxf>
-  </rcc>
-  <rfmt sheetId="2" sqref="A132:B132" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="700" sId="2">
-    <nc r="A133" t="inlineStr">
-      <is>
-        <t>AU-2</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="701" sId="2">
-    <nc r="B133" t="inlineStr">
-      <is>
-        <t>AUDIT EVENTS</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog21.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="702" sId="2" odxf="1" dxf="1">
-    <nc r="A110" t="inlineStr">
-      <is>
-        <t>AC-4</t>
-      </is>
-    </nc>
-    <odxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </odxf>
-    <ndxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </ndxf>
-  </rcc>
-  <rcc rId="703" sId="2" odxf="1" dxf="1">
-    <nc r="B110" t="inlineStr">
-      <is>
-        <t>INFORMATION FLOW ENFORCEMENT</t>
-      </is>
-    </nc>
-    <odxf>
-      <font>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </odxf>
-    <ndxf>
-      <font>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </ndxf>
-  </rcc>
-  <rfmt sheetId="2" sqref="A110:B110" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="2" sqref="A110:B110">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </rfmt>
-  <rcc rId="704" sId="2">
-    <nc r="A114" t="inlineStr">
-      <is>
-        <t>AC-6</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="705" sId="2">
-    <nc r="B114" t="inlineStr">
-      <is>
-        <t>LEAST PRIVILEGE</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="A114:B114" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="706" sId="2">
-    <nc r="A116" t="inlineStr">
-      <is>
-        <t xml:space="preserve">CM-8 </t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="707" sId="2" xfDxf="1" dxf="1">
-    <nc r="B116" t="inlineStr">
-      <is>
-        <t>INFORMATION SYSTEM COMPONENT INVENTORY</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </ndxf>
-  </rcc>
-  <rfmt sheetId="2" sqref="A116:B116" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="708" sId="2">
-    <nc r="A119" t="inlineStr">
-      <is>
-        <t>CM-7</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="709" sId="2">
-    <nc r="B119" t="inlineStr">
-      <is>
-        <t>LEAST FUNCTIONALITY</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="A119:B119" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="710" sId="2" xfDxf="1" dxf="1">
-    <nc r="B120" t="inlineStr">
-      <is>
-        <t>WIRELESS ACCESS | AUTHENTICATION AND ENCRYPTION</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </ndxf>
-  </rcc>
-  <rcc rId="711" sId="2">
-    <nc r="A120" t="inlineStr">
-      <is>
-        <t>AC-18(1)</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="A120:B120" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="712" sId="2" odxf="1" dxf="1">
-    <nc r="A121" t="inlineStr">
-      <is>
-        <t>AC-18(1)</t>
-      </is>
-    </nc>
-    <odxf>
-      <font>
-        <family val="2"/>
-      </font>
-    </odxf>
-    <ndxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </ndxf>
-  </rcc>
-  <rcc rId="713" sId="2" odxf="1" dxf="1">
-    <nc r="B121" t="inlineStr">
-      <is>
-        <t>WIRELESS ACCESS | AUTHENTICATION AND ENCRYPTION</t>
-      </is>
-    </nc>
-    <odxf>
-      <font>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-    </odxf>
-    <ndxf>
-      <font>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </ndxf>
-  </rcc>
-  <rcc rId="714" sId="2" odxf="1" dxf="1">
-    <nc r="A122" t="inlineStr">
-      <is>
-        <t>CM-7</t>
-      </is>
-    </nc>
-    <odxf>
-      <font>
-        <family val="2"/>
-      </font>
-    </odxf>
-    <ndxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </ndxf>
-  </rcc>
-  <rcc rId="715" sId="2" odxf="1" dxf="1">
-    <nc r="B122" t="inlineStr">
-      <is>
-        <t>LEAST FUNCTIONALITY</t>
-      </is>
-    </nc>
-    <odxf>
-      <font>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-    </odxf>
-    <ndxf>
-      <font>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </ndxf>
-  </rcc>
-  <rcc rId="716" sId="2" odxf="1" dxf="1">
-    <nc r="A123" t="inlineStr">
-      <is>
-        <t>CM-7</t>
-      </is>
-    </nc>
-    <odxf>
-      <font>
-        <family val="2"/>
-      </font>
-    </odxf>
-    <ndxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </ndxf>
-  </rcc>
-  <rcc rId="717" sId="2" odxf="1" dxf="1">
-    <nc r="B123" t="inlineStr">
-      <is>
-        <t>LEAST FUNCTIONALITY</t>
-      </is>
-    </nc>
-    <odxf>
-      <font>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-    </odxf>
-    <ndxf>
-      <font>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </ndxf>
-  </rcc>
-  <rcc rId="718" sId="2" odxf="1" dxf="1">
-    <nc r="A124" t="inlineStr">
-      <is>
-        <t>AC-4</t>
-      </is>
-    </nc>
-    <odxf>
-      <font>
-        <family val="2"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </odxf>
-    <ndxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </ndxf>
-  </rcc>
-  <rcc rId="719" sId="2" odxf="1" dxf="1">
-    <nc r="B124" t="inlineStr">
-      <is>
-        <t>INFORMATION FLOW ENFORCEMENT</t>
-      </is>
-    </nc>
-    <odxf>
-      <font>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </odxf>
-    <ndxf>
-      <font>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </ndxf>
-  </rcc>
-  <rcc rId="720" sId="2" xfDxf="1" dxf="1">
-    <nc r="B134" t="inlineStr">
-      <is>
-        <t>ACCOUNT MANAGEMENT</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </ndxf>
-  </rcc>
-  <rcc rId="721" sId="2">
-    <nc r="A134" t="inlineStr">
-      <is>
-        <t>AC-2</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="722" sId="2" xfDxf="1" dxf="1">
-    <nc r="B135" t="inlineStr">
-      <is>
-        <t>ACCOUNT MANAGEMENT | ACCOUNT MONITORING / ATYPICAL USAGE</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </ndxf>
-  </rcc>
-  <rcc rId="723" sId="2">
-    <nc r="A135" t="inlineStr">
-      <is>
-        <t>AC-2(12)</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="724" sId="2">
-    <nc r="B30" t="inlineStr">
-      <is>
-        <t>AUDIT REVIEW, ANALYSIS, AND REPORTING | INTEGRATION / SCANNING AND MONITORING CAPABILITIES</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="725" sId="2" xfDxf="1" dxf="1">
-    <oc r="B30" t="inlineStr">
-      <is>
-        <t>ACCOUNT MANAGEMENT | ACCOUNT MONITORING / ATYPICAL USAGE</t>
-      </is>
-    </oc>
-    <nc r="B30" t="inlineStr">
-      <is>
-        <t>AUDIT REVIEW, ANALYSIS, AND REPORTING | INTEGRATION / SCANNING AND MONITORING CAPABILITIES</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </ndxf>
-  </rcc>
-  <rcc rId="726" sId="2">
-    <oc r="A30" t="inlineStr">
-      <is>
-        <t>AC-2(12)</t>
-      </is>
-    </oc>
-    <nc r="A30" t="inlineStr">
-      <is>
-        <t>AU-6(5)</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="A30:B30" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="2" sqref="A133:B135" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="727" sId="2" xfDxf="1" dxf="1">
-    <nc r="B136" t="inlineStr">
-      <is>
-        <t>IDENTIFICATION AND AUTHENTICATION | NETWORK ACCESS TO PRIVILEGED ACCOUNTS</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </ndxf>
-  </rcc>
-  <rcc rId="728" sId="2">
-    <nc r="A136" t="inlineStr">
-      <is>
-        <t>IA-2(1)</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="A136:B136" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="729" sId="2">
-    <nc r="A137" t="inlineStr">
-      <is>
-        <t>IA-2</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="B137" start="0" length="0">
-    <dxf>
-      <font>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="730" sId="2">
-    <nc r="B137" t="inlineStr">
-      <is>
-        <t>IDENTIFICATION AND AUTHENTICATION</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="A137" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="731" sId="2">
-    <nc r="A138" t="inlineStr">
-      <is>
-        <t>SC-8</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="732" sId="2">
-    <nc r="B138" t="inlineStr">
-      <is>
-        <t>TRANSMISSION CONFIDENTIALITY AND INTEGRITY</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="A138:B138" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="733" sId="2">
-    <nc r="A139" t="inlineStr">
-      <is>
-        <t>SC-28</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="734" sId="2">
-    <nc r="B139" t="inlineStr">
-      <is>
-        <t>PROTECTION OF INFORMATION AT REST</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="A139:B139" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="735" sId="2">
-    <nc r="A148" t="inlineStr">
-      <is>
-        <t>SI-10</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="736" sId="2" odxf="1" dxf="1">
-    <nc r="B148" t="inlineStr">
-      <is>
-        <t>INFORMATION INPUT VALIDATION</t>
-      </is>
-    </nc>
-    <odxf>
-      <font>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-    </odxf>
-    <ndxf>
-      <font>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </ndxf>
-  </rcc>
-  <rfmt sheetId="2" sqref="A148" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="737" sId="2" odxf="1" dxf="1">
-    <nc r="A149" t="inlineStr">
-      <is>
-        <t>SI-10</t>
-      </is>
-    </nc>
-    <odxf>
-      <font>
-        <family val="2"/>
-      </font>
-    </odxf>
-    <ndxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </ndxf>
-  </rcc>
-  <rcc rId="738" sId="2" odxf="1" dxf="1">
-    <nc r="B149" t="inlineStr">
-      <is>
-        <t>INFORMATION INPUT VALIDATION</t>
-      </is>
-    </nc>
-    <odxf>
-      <font>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-    </odxf>
-    <ndxf>
-      <font>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </ndxf>
-  </rcc>
-  <rcc rId="739" sId="2">
-    <nc r="A150" t="inlineStr">
-      <is>
-        <t>RA-5</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="740" sId="2" odxf="1" dxf="1">
-    <nc r="B150" t="inlineStr">
-      <is>
-        <t>VULNERABILITY SCANNING</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </ndxf>
-  </rcc>
-  <rfmt sheetId="2" sqref="A150:B150" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="741" sId="2" xfDxf="1" dxf="1">
-    <nc r="B151" t="inlineStr">
-      <is>
-        <t>ERROR HANDLING</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </ndxf>
-  </rcc>
-  <rcc rId="742" sId="2">
-    <nc r="A151" t="inlineStr">
-      <is>
-        <t>SI-11</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="A151:B151" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="743" sId="2">
-    <nc r="A153" t="inlineStr">
-      <is>
-        <t>CM-6</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="744" sId="2">
-    <nc r="B153" t="inlineStr">
-      <is>
-        <t>CONFIGURATION SETTINGS</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="A153:B153" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="745" sId="2" xfDxf="1" dxf="1">
-    <nc r="B154" t="inlineStr">
-      <is>
-        <t>ROLE-BASED SECURITY TRAINING</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </ndxf>
-  </rcc>
-  <rcc rId="746" sId="2">
-    <nc r="A154" t="inlineStr">
-      <is>
-        <t>AT-3</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="A154:B154" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="747" sId="2">
-    <nc r="A152" t="inlineStr">
-      <is>
-        <t>AC-6</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="748" sId="2">
-    <nc r="B152" t="inlineStr">
-      <is>
-        <t>LEAST PRIVILEGE</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="A152:B152" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="749" sId="2">
-    <nc r="A155" t="inlineStr">
-      <is>
-        <t>CM-7</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="750" sId="2">
-    <nc r="B155" t="inlineStr">
-      <is>
-        <t>LEAST FUNCTIONALITY</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="A155:B155" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcv guid="{9FD8CC1C-6420-44A1-A370-C19CD963FBCC}" action="delete"/>
-  <rdn rId="0" localSheetId="2" customView="1" name="Z_9FD8CC1C_6420_44A1_A370_C19CD963FBCC_.wvu.PrintArea" hidden="1" oldHidden="1">
-    <formula>'VER 6.1 Controls'!$C$3:$E$172</formula>
-    <oldFormula>'VER 6.1 Controls'!$C$3:$E$172</oldFormula>
-  </rdn>
-  <rdn rId="0" localSheetId="2" customView="1" name="Z_9FD8CC1C_6420_44A1_A370_C19CD963FBCC_.wvu.FilterData" hidden="1" oldHidden="1">
-    <formula>'VER 6.1 Controls'!$A$3:$H$172</formula>
-  </rdn>
-  <rcv guid="{9FD8CC1C-6420-44A1-A370-C19CD963FBCC}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog22.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="753" sId="2" xfDxf="1" dxf="1">
-    <nc r="B87" t="inlineStr">
-      <is>
-        <t>SYSTEM INTERCONNECTIONS | RESTRICTIONS ON EXTERNAL SYSTEM CONNECTIONS</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </ndxf>
-  </rcc>
-  <rcc rId="754" sId="2">
-    <nc r="A87" t="inlineStr">
-      <is>
-        <t>CA-3(5)</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="A87:B87" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="755" sId="2" xfDxf="1" dxf="1">
-    <nc r="B88" t="inlineStr">
-      <is>
-        <t>INFORMATION SYSTEM MONITORING | AUTOMATED TOOLS FOR REAL-TIME ANALYSIS</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </ndxf>
-  </rcc>
-  <rcc rId="756" sId="2">
-    <nc r="A88" t="inlineStr">
-      <is>
-        <t>SI-4(2)</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="A88:B88" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="757" sId="2" xfDxf="1" dxf="1">
-    <nc r="B89" t="inlineStr">
-      <is>
-        <t>INFORMATION SYSTEM MONITORING | SYSTEM-WIDE INTRUSION DETECTION SYSTEM</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </ndxf>
-  </rcc>
-  <rcc rId="758" sId="2">
-    <nc r="A89" t="inlineStr">
-      <is>
-        <t>SI-4(1)</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="A89:B89" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="759" sId="2">
-    <nc r="A90" t="inlineStr">
-      <is>
-        <t>SI-4</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="B90" start="0" length="0">
-    <dxf>
-      <font>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="760" sId="2">
-    <nc r="B90" t="inlineStr">
-      <is>
-        <t>INFORMATION SYSTEM MONITORING</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="A90" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="761" sId="2" xfDxf="1" dxf="1">
-    <nc r="B91" t="inlineStr">
-      <is>
-        <t>BOUNDARY PROTECTION | ROUTE TRAFFIC TO AUTHENTICATED PROXY SERVERS</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </ndxf>
-  </rcc>
-  <rcc rId="762" sId="2">
-    <nc r="A91" t="inlineStr">
-      <is>
-        <t>SC-7(8)</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="A91:B91" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="2" xfDxf="1" sqref="B92" start="0" length="0">
-    <dxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-  </rfmt>
-  <rcc rId="763" sId="2">
-    <nc r="B92" t="inlineStr">
-      <is>
-        <t>IDENTIFICATION AND AUTHENTICATION | NETWORK ACCESS TO PRIVILEGED ACCOUNTS
-IDENTIFICATION AND AUTHENTICATION | NETWORK ACCESS TO NON-PRIVILEGED ACCOUNTS</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="764" sId="2" odxf="1" dxf="1">
-    <nc r="A92" t="inlineStr">
-      <is>
-        <t>IA-2(1)
-IA-2(2)</t>
-      </is>
-    </nc>
-    <odxf>
-      <alignment wrapText="0"/>
-    </odxf>
-    <ndxf>
-      <alignment wrapText="1"/>
-    </ndxf>
-  </rcc>
-  <rfmt sheetId="2" sqref="A92:B92" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="765" sId="2" xfDxf="1" dxf="1">
-    <nc r="B93" t="inlineStr">
-      <is>
-        <t>DEVICE IDENTIFICATION AND AUTHENTICATION | DEVICE ATTESTATION</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </ndxf>
-  </rcc>
-  <rcc rId="766" sId="2">
-    <nc r="A93" t="inlineStr">
-      <is>
-        <t>IA-3(4)</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="A93:B93" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="767" sId="2" xfDxf="1" dxf="1">
-    <nc r="B94" t="inlineStr">
-      <is>
-        <t>INFORMATION SYSTEM MONITORING</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </ndxf>
-  </rcc>
-  <rcc rId="768" sId="2">
-    <nc r="A94" t="inlineStr">
-      <is>
-        <t>SI-4</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="A94:B94" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="769" sId="2" xfDxf="1" dxf="1">
-    <nc r="B95" t="inlineStr">
-      <is>
-        <t>INFORMATION SYSTEM MONITORING | ANALYZE COMMUNICATIONS TRAFFIC ANOMALIES</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </ndxf>
-  </rcc>
-  <rfmt sheetId="2" sqref="A95" start="0" length="0">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="770" sId="2">
-    <nc r="A95" t="inlineStr">
-      <is>
-        <t>SI-4(11)</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="B95" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="771" sId="2" xfDxf="1" dxf="1">
-    <nc r="B96" t="inlineStr">
-      <is>
-        <t>INFORMATION SYSTEM MONITORING | ANALYZE TRAFFIC / COVERT EXFILTRATION</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </ndxf>
-  </rcc>
-  <rfmt sheetId="2" sqref="A96" start="0" length="0">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="772" sId="2">
-    <nc r="A96" t="inlineStr">
-      <is>
-        <t>SI-4(18)</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="B96" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog23.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="773" sId="2" xfDxf="1" dxf="1">
-    <nc r="B98" t="inlineStr">
-      <is>
-        <t>PRIVACY IMPACT AND RISK ASSESSMENT</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </ndxf>
-  </rcc>
-  <rcc rId="774" sId="2">
-    <nc r="A98" t="inlineStr">
-      <is>
-        <t>AR-2</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="A98:B98" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rfmt sheetId="2" sqref="A99:B99" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="775" sId="2" xfDxf="1" dxf="1">
-    <nc r="B99" t="inlineStr">
-      <is>
-        <t>PROTECTION OF INFORMATION AT REST | CRYPTOGRAPHIC PROTECTION</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </ndxf>
-  </rcc>
-  <rcc rId="776" sId="2">
-    <nc r="A99" t="inlineStr">
-      <is>
-        <t>SC-28(1)</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="777" sId="2" xfDxf="1" dxf="1">
-    <nc r="B100" t="inlineStr">
-      <is>
-        <t>BOUNDARY PROTECTION | PREVENT UNAUTHORIZED EXFILTRATION</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </ndxf>
-  </rcc>
-  <rcc rId="778" sId="2">
-    <nc r="A100" t="inlineStr">
-      <is>
-        <t>SC-7(10)</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="779" sId="2" xfDxf="1" dxf="1">
-    <nc r="B101" t="inlineStr">
-      <is>
-        <t>MINIMIZATION OF PERSONALLY IDENTIFIABLE INFORMATION | LOCATE / REMOVE / REDACT / ANONYMIZE PII</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </ndxf>
-  </rcc>
-  <rcc rId="780" sId="2">
-    <nc r="A101" t="inlineStr">
-      <is>
-        <t>DM-1(1)</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="781" sId="2">
-    <nc r="A102" t="inlineStr">
-      <is>
-        <t>MP-4</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="782" sId="2">
-    <nc r="B102" t="inlineStr">
-      <is>
-        <t>MEDIA STORAGE</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="783" sId="2" xfDxf="1" dxf="1">
-    <nc r="B104" t="inlineStr">
-      <is>
-        <t>INFORMATION FLOW ENFORCEMENT | CONTENT CHECK ENCRYPTED INFORMATION</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </ndxf>
-  </rcc>
-  <rcc rId="784" sId="2">
-    <nc r="A104" t="inlineStr">
-      <is>
-        <t>AC-4(4)</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="785" sId="2" xfDxf="1" dxf="1">
-    <nc r="B103" t="inlineStr">
-      <is>
-        <t>INFORMATION SYSTEM MONITORING | INBOUND AND OUTBOUND COMMUNICATIONS TRAFFIC</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </ndxf>
-  </rcc>
-  <rcc rId="786" sId="2">
-    <nc r="A103" t="inlineStr">
-      <is>
-        <t>SI-4(4)</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog24.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rfmt sheetId="2" sqref="A100:B104" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="787" sId="2" xfDxf="1" dxf="1">
-    <nc r="B105" t="inlineStr">
-      <is>
-        <t>BOUNDARY PROTECTION | PREVENT UNAUTHORIZED EXFILTRATION</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </ndxf>
-  </rcc>
-  <rcc rId="788" sId="2">
-    <nc r="A105" t="inlineStr">
-      <is>
-        <t>SC-7(10)</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="A105:B106" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcv guid="{9FD8CC1C-6420-44A1-A370-C19CD963FBCC}" action="delete"/>
-  <rdn rId="0" localSheetId="2" customView="1" name="Z_9FD8CC1C_6420_44A1_A370_C19CD963FBCC_.wvu.PrintArea" hidden="1" oldHidden="1">
-    <formula>'VER 6.1 Controls'!$C$3:$E$172</formula>
-    <oldFormula>'VER 6.1 Controls'!$C$3:$E$172</oldFormula>
-  </rdn>
-  <rdn rId="0" localSheetId="2" customView="1" name="Z_9FD8CC1C_6420_44A1_A370_C19CD963FBCC_.wvu.FilterData" hidden="1" oldHidden="1">
-    <formula>'VER 6.1 Controls'!$A$3:$H$172</formula>
-    <oldFormula>'VER 6.1 Controls'!$A$3:$H$172</oldFormula>
-  </rdn>
-  <rcv guid="{9FD8CC1C-6420-44A1-A370-C19CD963FBCC}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog25.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="791" sId="2">
-    <nc r="A106" t="inlineStr">
-      <is>
-        <t>AC-3 (3)</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="792" sId="2">
-    <nc r="B106" t="inlineStr">
-      <is>
-        <t>ACCESS ENFORCEMENT | MANDATORY ACCESS CONTROL</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcv guid="{9FD8CC1C-6420-44A1-A370-C19CD963FBCC}" action="delete"/>
-  <rdn rId="0" localSheetId="2" customView="1" name="Z_9FD8CC1C_6420_44A1_A370_C19CD963FBCC_.wvu.PrintArea" hidden="1" oldHidden="1">
-    <formula>'VER 6.1 Controls'!$C$3:$E$172</formula>
-    <oldFormula>'VER 6.1 Controls'!$C$3:$E$172</oldFormula>
-  </rdn>
-  <rdn rId="0" localSheetId="2" customView="1" name="Z_9FD8CC1C_6420_44A1_A370_C19CD963FBCC_.wvu.FilterData" hidden="1" oldHidden="1">
-    <formula>'VER 6.1 Controls'!$A$3:$H$172</formula>
-    <oldFormula>'VER 6.1 Controls'!$A$3:$H$172</oldFormula>
-  </rdn>
-  <rcv guid="{9FD8CC1C-6420-44A1-A370-C19CD963FBCC}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog26.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="795" sId="2">
-    <oc r="B92" t="inlineStr">
-      <is>
-        <t>IDENTIFICATION AND AUTHENTICATION | NETWORK ACCESS TO PRIVILEGED ACCOUNTS
-IDENTIFICATION AND AUTHENTICATION | NETWORK ACCESS TO NON-PRIVILEGED ACCOUNTS</t>
-      </is>
-    </oc>
-    <nc r="B92" t="inlineStr">
-      <is>
-        <t>IDENTIFICATION AND AUTHENTICATION | NETWORK ACCESS TO PRIVILEGED ACCOUNTS</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="796" sId="2">
-    <oc r="A92" t="inlineStr">
-      <is>
-        <t>IA-2(1)
-IA-2(2)</t>
-      </is>
-    </oc>
-    <nc r="A92" t="inlineStr">
-      <is>
-        <t>IA-2(1)</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcv guid="{9FD8CC1C-6420-44A1-A370-C19CD963FBCC}" action="delete"/>
-  <rdn rId="0" localSheetId="2" customView="1" name="Z_9FD8CC1C_6420_44A1_A370_C19CD963FBCC_.wvu.PrintArea" hidden="1" oldHidden="1">
-    <formula>'VER 6.1 Controls'!$C$3:$E$172</formula>
-    <oldFormula>'VER 6.1 Controls'!$C$3:$E$172</oldFormula>
-  </rdn>
-  <rdn rId="0" localSheetId="2" customView="1" name="Z_9FD8CC1C_6420_44A1_A370_C19CD963FBCC_.wvu.FilterData" hidden="1" oldHidden="1">
-    <formula>'VER 6.1 Controls'!$A$3:$H$172</formula>
-    <oldFormula>'VER 6.1 Controls'!$A$3:$H$172</oldFormula>
-  </rdn>
-  <rcv guid="{9FD8CC1C-6420-44A1-A370-C19CD963FBCC}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog27.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="799" sId="2" xfDxf="1" dxf="1">
-    <nc r="B141" t="inlineStr">
-      <is>
-        <t>ROLE-BASED SECURITY TRAINING</t>
-      </is>
-    </nc>
-    <ndxf>
-      <font>
-        <b/>
-        <sz val="9"/>
-        <family val="2"/>
-      </font>
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </ndxf>
-  </rcc>
-  <rcc rId="800" sId="2">
-    <nc r="A141" t="inlineStr">
-      <is>
-        <t>AT-3</t>
-      </is>
-    </nc>
-  </rcc>
-  <rfmt sheetId="2" sqref="A141:B145" start="0" length="2147483647">
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-        <family val="2"/>
-      </font>
-    </dxf>
-  </rfmt>
-  <rcc rId="801" sId="2">
-    <nc r="A142" t="inlineStr">
-      <is>
-        <t>AT-3</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="802" sId="2">
-    <nc r="B142" t="inlineStr">
-      <is>
-        <t>ROLE-BASED SECURITY TRAINING</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="803" sId="2">
-    <nc r="A143" t="inlineStr">
-      <is>
-        <t>AT-3</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="804" sId="2">
-    <nc r="B143" t="inlineStr">
-      <is>
-        <t>ROLE-BASED SECURITY TRAINING</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="805" sId="2">
-    <nc r="A144" t="inlineStr">
-      <is>
-        <t>AT-3</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="806" sId="2">
-    <nc r="B144" t="inlineStr">
-      <is>
-        <t>ROLE-BASED SECURITY TRAINING</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="807" sId="2">
-    <nc r="A145" t="inlineStr">
-      <is>
-        <t>AT-3</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="808" sId="2">
-    <nc r="B145" t="inlineStr">
-      <is>
-        <t>ROLE-BASED SECURITY TRAINING</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
 </file>
 
 <file path=xl/revisions/revisionLog28.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6622,131 +2838,10 @@
 </revisions>
 </file>
 
-<file path=xl/revisions/revisionLog3.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="563" sId="2">
-    <oc r="A67" t="inlineStr">
-      <is>
-        <t>CM-7</t>
-      </is>
-    </oc>
-    <nc r="A67" t="inlineStr">
-      <is>
-        <t>CM-7 (1)</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog4.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="564" sId="2">
-    <nc r="H67" t="inlineStr">
-      <is>
-        <t>(4) UNAUTHORIZED SOFWTARE /BLACKLISTING</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog5.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="565" sId="2">
-    <nc r="A108" t="inlineStr">
-      <is>
-        <t>AC-3 (3) for autohrized indicvualdal part</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcv guid="{166C989B-D112-4FBE-9337-483856443AEC}" action="delete"/>
-  <rdn rId="0" localSheetId="2" customView="1" name="Z_166C989B_D112_4FBE_9337_483856443AEC_.wvu.PrintArea" hidden="1" oldHidden="1">
-    <formula>'VER 6.1 Controls'!$C$3:$E$172</formula>
-    <oldFormula>'VER 6.1 Controls'!$C$3:$E$172</oldFormula>
-  </rdn>
-  <rcv guid="{166C989B-D112-4FBE-9337-483856443AEC}" action="add"/>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog6.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="567" sId="2">
-    <oc r="A108" t="inlineStr">
-      <is>
-        <t>AC-3 (3) for autohrized indicvualdal part</t>
-      </is>
-    </oc>
-    <nc r="A108" t="inlineStr">
-      <is>
-        <t>AC-4 for information flow segmenation,  AC-3 (3) for autohrized indicvualdal part</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog7.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="568" sId="2">
-    <oc r="A108" t="inlineStr">
-      <is>
-        <t>AC-4 for information flow segmenation,  AC-3 (3) for autohrized indicvualdal part</t>
-      </is>
-    </oc>
-    <nc r="A108" t="inlineStr">
-      <is>
-        <t>AC-4,  AC-3 (3)</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog8.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="569" sId="2">
-    <oc r="A108" t="inlineStr">
-      <is>
-        <t>AC-4,  AC-3 (3)</t>
-      </is>
-    </oc>
-    <nc r="A108" t="inlineStr">
-      <is>
-        <t>AC-4,  AC-3 (3), SC-7</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
-<file path=xl/revisions/revisionLog9.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="570" sId="2">
-    <oc r="A108" t="inlineStr">
-      <is>
-        <t>AC-4,  AC-3 (3), SC-7</t>
-      </is>
-    </oc>
-    <nc r="A108" t="inlineStr">
-      <is>
-        <t>AC-4</t>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="571" sId="2">
-    <nc r="H108" t="inlineStr">
-      <is>
-        <t>Others that could be considered if not related AC-3 (3), SC-7.</t>
-      </is>
-    </nc>
-  </rcc>
-</revisions>
-</file>
-
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="1">
+<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="2">
   <userInfo guid="{6663B3B2-0172-4D31-B8DB-D15A051B9192}" name="Aronne, Eugene J." id="-567976790" dateTime="2017-09-21T12:09:09"/>
+  <userInfo guid="{2F8F7620-4C4F-A040-A1DD-B07BF2744515}" name="Microsoft Office User" id="-296998420" dateTime="2017-10-30T20:24:54"/>
 </users>
 </file>
 

</xml_diff>